<commit_message>
changes the GDD to make it clearer
</commit_message>
<xml_diff>
--- a/documents/Game data.xlsx
+++ b/documents/Game data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naomi\Desktop\UNI\Aventale Interactive\aventale-interactive-gam130\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dm1\aventale-interactive-gam130\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DFB759-3953-4A63-B768-6D04284E196B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DB4328-C850-404D-948D-6ACD007FEB3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B55EC6BF-FA38-47AF-9968-4D4850AC5ACB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B55EC6BF-FA38-47AF-9968-4D4850AC5ACB}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="2" r:id="rId1"/>
@@ -448,10 +448,10 @@
     <t>Cap amount of Player's units are on board at once.</t>
   </si>
   <si>
-    <t>Archers can be placed into the fort. Allows fort to retaliate as well as attack enemy units in range.</t>
-  </si>
-  <si>
     <t>Max amount units on board:</t>
+  </si>
+  <si>
+    <t>1 Archer can be placed into each fort/Castle. Allows fort/castle to retaliate as well as attack enemy units in range.</t>
   </si>
 </sst>
 </file>
@@ -770,31 +770,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -804,9 +807,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="19">
         <v>10</v>
@@ -1264,7 +1264,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>2</v>
@@ -1281,7 +1281,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>0</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B36" s="35"/>
       <c r="C36" s="35"/>
@@ -1506,25 +1506,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="69" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="70" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -1545,13 +1545,13 @@
       <c r="F3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
     </row>
@@ -1563,13 +1563,13 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
       <c r="M4" t="s">
         <v>37</v>
       </c>
@@ -1599,17 +1599,17 @@
       <c r="F5" s="15">
         <v>10</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="H5" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="66" t="s">
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="66"/>
+      <c r="N5" s="61"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -1630,17 +1630,17 @@
       <c r="F6" s="16">
         <v>15</v>
       </c>
-      <c r="H6" s="65" t="s">
+      <c r="H6" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="66" t="s">
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="66"/>
+      <c r="N6" s="61"/>
       <c r="O6" s="35" t="s">
         <v>41</v>
       </c>
@@ -1669,13 +1669,13 @@
       <c r="F7" s="17">
         <v>25</v>
       </c>
-      <c r="H7" s="65" t="s">
+      <c r="H7" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
       <c r="M7" t="s">
         <v>49</v>
       </c>
@@ -1710,10 +1710,10 @@
       <c r="N8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S8" s="68" t="s">
+      <c r="S8" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T8" s="68"/>
+      <c r="T8" s="63"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1728,22 +1728,22 @@
       <c r="J9" s="37"/>
       <c r="K9" s="32"/>
       <c r="L9" s="37"/>
-      <c r="N9" s="62" t="s">
+      <c r="N9" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62" t="s">
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
-      <c r="X9" s="62"/>
-      <c r="Y9" s="62"/>
+      <c r="T9" s="60"/>
+      <c r="U9" s="60"/>
+      <c r="V9" s="60"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="60"/>
+      <c r="Y9" s="60"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1769,22 +1769,22 @@
       <c r="J10" s="32"/>
       <c r="K10" s="37"/>
       <c r="L10" s="32"/>
-      <c r="N10" s="62" t="s">
+      <c r="N10" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62" t="s">
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="T10" s="62"/>
-      <c r="U10" s="62"/>
-      <c r="V10" s="62"/>
-      <c r="W10" s="62"/>
-      <c r="X10" s="62"/>
-      <c r="Y10" s="62"/>
+      <c r="T10" s="60"/>
+      <c r="U10" s="60"/>
+      <c r="V10" s="60"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1810,20 +1810,20 @@
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="37"/>
-      <c r="N11" s="62" t="s">
+      <c r="N11" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="62"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="62"/>
-      <c r="V11" s="62"/>
-      <c r="W11" s="62"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="60"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="60"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
@@ -1849,20 +1849,20 @@
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="32"/>
-      <c r="N12" s="62" t="s">
+      <c r="N12" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="62"/>
-      <c r="T12" s="62"/>
-      <c r="U12" s="62"/>
-      <c r="V12" s="62"/>
-      <c r="W12" s="62"/>
-      <c r="X12" s="62"/>
-      <c r="Y12" s="62"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -1888,18 +1888,18 @@
       <c r="J13" s="37"/>
       <c r="K13" s="32"/>
       <c r="L13" s="37"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="62"/>
-      <c r="R13" s="62"/>
-      <c r="S13" s="62"/>
-      <c r="T13" s="62"/>
-      <c r="U13" s="62"/>
-      <c r="V13" s="62"/>
-      <c r="W13" s="62"/>
-      <c r="X13" s="62"/>
-      <c r="Y13" s="62"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="60"/>
+      <c r="V13" s="60"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="60"/>
+      <c r="Y13" s="60"/>
     </row>
     <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
@@ -1920,13 +1920,13 @@
       <c r="F15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="68" t="s">
+      <c r="H15" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
       <c r="M15" s="33"/>
       <c r="N15" s="33"/>
     </row>
@@ -1938,13 +1938,13 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="H16" s="63" t="s">
+      <c r="H16" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
       <c r="M16" s="40" t="s">
         <v>51</v>
       </c>
@@ -1974,17 +1974,17 @@
       <c r="F17" s="15">
         <v>10</v>
       </c>
-      <c r="H17" s="65" t="s">
+      <c r="H17" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="66" t="s">
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="66"/>
+      <c r="N17" s="61"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -2005,17 +2005,17 @@
       <c r="F18" s="16">
         <v>15</v>
       </c>
-      <c r="H18" s="63" t="s">
+      <c r="H18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63"/>
-      <c r="M18" s="66" t="s">
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="66"/>
+      <c r="N18" s="61"/>
       <c r="O18" s="39" t="s">
         <v>53</v>
       </c>
@@ -2044,13 +2044,13 @@
       <c r="F19" s="42">
         <v>25</v>
       </c>
-      <c r="H19" s="63" t="s">
+      <c r="H19" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="63"/>
-      <c r="L19" s="63"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
       <c r="M19" s="40" t="s">
         <v>52</v>
       </c>
@@ -2085,10 +2085,10 @@
       <c r="N20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S20" s="68" t="s">
+      <c r="S20" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T20" s="68"/>
+      <c r="T20" s="63"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2103,22 +2103,22 @@
       <c r="J21" s="37"/>
       <c r="K21" s="32"/>
       <c r="L21" s="37"/>
-      <c r="N21" s="62" t="s">
+      <c r="N21" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="O21" s="62"/>
-      <c r="P21" s="62"/>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62"/>
-      <c r="S21" s="62" t="s">
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="T21" s="62"/>
-      <c r="U21" s="62"/>
-      <c r="V21" s="62"/>
-      <c r="W21" s="62"/>
-      <c r="X21" s="62"/>
-      <c r="Y21" s="62"/>
+      <c r="T21" s="60"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="60"/>
+      <c r="Y21" s="60"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
@@ -2144,22 +2144,22 @@
       <c r="J22" s="31"/>
       <c r="K22" s="37"/>
       <c r="L22" s="32"/>
-      <c r="N22" s="62" t="s">
+      <c r="N22" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="O22" s="62"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="62"/>
-      <c r="R22" s="62"/>
-      <c r="S22" s="62" t="s">
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="60"/>
+      <c r="S22" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="T22" s="62"/>
-      <c r="U22" s="62"/>
-      <c r="V22" s="62"/>
-      <c r="W22" s="62"/>
-      <c r="X22" s="62"/>
-      <c r="Y22" s="62"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="60"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -2185,22 +2185,22 @@
       <c r="J23" s="31"/>
       <c r="K23" s="38"/>
       <c r="L23" s="37"/>
-      <c r="N23" s="62" t="s">
+      <c r="N23" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62" t="s">
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="T23" s="62"/>
-      <c r="U23" s="62"/>
-      <c r="V23" s="62"/>
-      <c r="W23" s="62"/>
-      <c r="X23" s="62"/>
-      <c r="Y23" s="62"/>
+      <c r="T23" s="60"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="60"/>
+      <c r="W23" s="60"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
@@ -2226,20 +2226,20 @@
       <c r="J24" s="38"/>
       <c r="K24" s="37"/>
       <c r="L24" s="32"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="62"/>
-      <c r="R24" s="62"/>
-      <c r="S24" s="62" t="s">
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="T24" s="62"/>
-      <c r="U24" s="62"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="62"/>
-      <c r="X24" s="62"/>
-      <c r="Y24" s="62"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="60"/>
+      <c r="W24" s="60"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -2265,20 +2265,20 @@
       <c r="J25" s="37"/>
       <c r="K25" s="32"/>
       <c r="L25" s="37"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="62"/>
-      <c r="R25" s="62"/>
-      <c r="S25" s="62" t="s">
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="T25" s="62"/>
-      <c r="U25" s="62"/>
-      <c r="V25" s="62"/>
-      <c r="W25" s="62"/>
-      <c r="X25" s="62"/>
-      <c r="Y25" s="62"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="60"/>
+      <c r="V25" s="60"/>
+      <c r="W25" s="60"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
     </row>
     <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
@@ -2299,13 +2299,13 @@
       <c r="F27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="68" t="s">
+      <c r="H27" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
       <c r="M27" s="33"/>
       <c r="N27" s="33"/>
     </row>
@@ -2317,13 +2317,13 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="H28" s="67" t="s">
+      <c r="H28" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="68"/>
       <c r="M28" s="43" t="s">
         <v>51</v>
       </c>
@@ -2354,17 +2354,17 @@
       <c r="F29" s="15">
         <v>10</v>
       </c>
-      <c r="H29" s="67" t="s">
+      <c r="H29" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="72" t="s">
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N29" s="72"/>
+      <c r="N29" s="69"/>
       <c r="O29" s="43"/>
       <c r="P29" s="43"/>
     </row>
@@ -2387,17 +2387,17 @@
       <c r="F30" s="16">
         <v>15</v>
       </c>
-      <c r="H30" s="67" t="s">
+      <c r="H30" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="L30" s="67"/>
-      <c r="M30" s="72" t="s">
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="N30" s="72"/>
+      <c r="N30" s="69"/>
       <c r="O30" s="44" t="s">
         <v>53</v>
       </c>
@@ -2426,13 +2426,13 @@
       <c r="F31" s="41">
         <v>20</v>
       </c>
-      <c r="H31" s="63" t="s">
+      <c r="H31" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="63"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
       <c r="M31" s="40" t="s">
         <v>64</v>
       </c>
@@ -2470,10 +2470,10 @@
       <c r="N32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S32" s="68" t="s">
+      <c r="S32" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T32" s="68"/>
+      <c r="T32" s="63"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2488,22 +2488,22 @@
       <c r="J33" s="37"/>
       <c r="K33" s="32"/>
       <c r="L33" s="37"/>
-      <c r="N33" s="62" t="s">
+      <c r="N33" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="O33" s="62"/>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="62"/>
-      <c r="R33" s="62"/>
-      <c r="S33" s="62" t="s">
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="T33" s="62"/>
-      <c r="U33" s="62"/>
-      <c r="V33" s="62"/>
-      <c r="W33" s="62"/>
-      <c r="X33" s="62"/>
-      <c r="Y33" s="62"/>
+      <c r="T33" s="60"/>
+      <c r="U33" s="60"/>
+      <c r="V33" s="60"/>
+      <c r="W33" s="60"/>
+      <c r="X33" s="60"/>
+      <c r="Y33" s="60"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
@@ -2529,22 +2529,22 @@
       <c r="J34" s="31"/>
       <c r="K34" s="37"/>
       <c r="L34" s="32"/>
-      <c r="N34" s="62" t="s">
+      <c r="N34" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="62"/>
-      <c r="S34" s="62" t="s">
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="T34" s="62"/>
-      <c r="U34" s="62"/>
-      <c r="V34" s="62"/>
-      <c r="W34" s="62"/>
-      <c r="X34" s="62"/>
-      <c r="Y34" s="62"/>
+      <c r="T34" s="60"/>
+      <c r="U34" s="60"/>
+      <c r="V34" s="60"/>
+      <c r="W34" s="60"/>
+      <c r="X34" s="60"/>
+      <c r="Y34" s="60"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
@@ -2570,20 +2570,20 @@
       <c r="J35" s="31"/>
       <c r="K35" s="38"/>
       <c r="L35" s="37"/>
-      <c r="N35" s="62"/>
-      <c r="O35" s="62"/>
-      <c r="P35" s="62"/>
-      <c r="Q35" s="62"/>
-      <c r="R35" s="62"/>
-      <c r="S35" s="62" t="s">
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="T35" s="62"/>
-      <c r="U35" s="62"/>
-      <c r="V35" s="62"/>
-      <c r="W35" s="62"/>
-      <c r="X35" s="62"/>
-      <c r="Y35" s="62"/>
+      <c r="T35" s="60"/>
+      <c r="U35" s="60"/>
+      <c r="V35" s="60"/>
+      <c r="W35" s="60"/>
+      <c r="X35" s="60"/>
+      <c r="Y35" s="60"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
@@ -2609,18 +2609,18 @@
       <c r="J36" s="38"/>
       <c r="K36" s="37"/>
       <c r="L36" s="32"/>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
-      <c r="Q36" s="62"/>
-      <c r="R36" s="62"/>
-      <c r="S36" s="62"/>
-      <c r="T36" s="62"/>
-      <c r="U36" s="62"/>
-      <c r="V36" s="62"/>
-      <c r="W36" s="62"/>
-      <c r="X36" s="62"/>
-      <c r="Y36" s="62"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="60"/>
+      <c r="U36" s="60"/>
+      <c r="V36" s="60"/>
+      <c r="W36" s="60"/>
+      <c r="X36" s="60"/>
+      <c r="Y36" s="60"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
@@ -2646,18 +2646,18 @@
       <c r="J37" s="37"/>
       <c r="K37" s="32"/>
       <c r="L37" s="37"/>
-      <c r="N37" s="62"/>
-      <c r="O37" s="62"/>
-      <c r="P37" s="62"/>
-      <c r="Q37" s="62"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="62"/>
-      <c r="T37" s="62"/>
-      <c r="U37" s="62"/>
-      <c r="V37" s="62"/>
-      <c r="W37" s="62"/>
-      <c r="X37" s="62"/>
-      <c r="Y37" s="62"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
+      <c r="U37" s="60"/>
+      <c r="V37" s="60"/>
+      <c r="W37" s="60"/>
+      <c r="X37" s="60"/>
+      <c r="Y37" s="60"/>
     </row>
     <row r="39" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
@@ -2675,13 +2675,13 @@
       <c r="E39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="68" t="s">
+      <c r="H39" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="68"/>
-      <c r="L39" s="68"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
       <c r="M39" s="33"/>
       <c r="N39" s="33"/>
     </row>
@@ -2693,13 +2693,13 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="H40" s="65" t="s">
+      <c r="H40" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="I40" s="65"/>
-      <c r="J40" s="65"/>
-      <c r="K40" s="65"/>
-      <c r="L40" s="65"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="64"/>
+      <c r="L40" s="64"/>
       <c r="M40" t="s">
         <v>70</v>
       </c>
@@ -2729,17 +2729,17 @@
       <c r="E41" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="65" t="s">
+      <c r="H41" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="I41" s="65"/>
-      <c r="J41" s="65"/>
-      <c r="K41" s="65"/>
-      <c r="L41" s="65"/>
-      <c r="M41" s="66" t="s">
+      <c r="I41" s="64"/>
+      <c r="J41" s="64"/>
+      <c r="K41" s="64"/>
+      <c r="L41" s="64"/>
+      <c r="M41" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="N41" s="66"/>
+      <c r="N41" s="61"/>
       <c r="O41" t="s">
         <v>72</v>
       </c>
@@ -2779,13 +2779,13 @@
       <c r="E43" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H43" s="67" t="s">
+      <c r="H43" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="I43" s="67"/>
-      <c r="J43" s="67"/>
-      <c r="K43" s="67"/>
-      <c r="L43" s="67"/>
+      <c r="I43" s="68"/>
+      <c r="J43" s="68"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="68"/>
       <c r="M43" s="43" t="s">
         <v>64</v>
       </c>
@@ -2818,10 +2818,10 @@
       <c r="N44" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S44" s="68" t="s">
+      <c r="S44" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T44" s="68"/>
+      <c r="T44" s="63"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -2836,22 +2836,22 @@
       <c r="J45" s="37"/>
       <c r="K45" s="32"/>
       <c r="L45" s="37"/>
-      <c r="N45" s="62" t="s">
+      <c r="N45" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="O45" s="62"/>
-      <c r="P45" s="62"/>
-      <c r="Q45" s="62"/>
-      <c r="R45" s="62"/>
-      <c r="S45" s="62" t="s">
+      <c r="O45" s="60"/>
+      <c r="P45" s="60"/>
+      <c r="Q45" s="60"/>
+      <c r="R45" s="60"/>
+      <c r="S45" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="T45" s="62"/>
-      <c r="U45" s="62"/>
-      <c r="V45" s="62"/>
-      <c r="W45" s="62"/>
-      <c r="X45" s="62"/>
-      <c r="Y45" s="62"/>
+      <c r="T45" s="60"/>
+      <c r="U45" s="60"/>
+      <c r="V45" s="60"/>
+      <c r="W45" s="60"/>
+      <c r="X45" s="60"/>
+      <c r="Y45" s="60"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
@@ -2874,22 +2874,22 @@
       <c r="J46" s="31"/>
       <c r="K46" s="37"/>
       <c r="L46" s="32"/>
-      <c r="N46" s="62" t="s">
+      <c r="N46" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="O46" s="62"/>
-      <c r="P46" s="62"/>
-      <c r="Q46" s="62"/>
-      <c r="R46" s="62"/>
-      <c r="S46" s="62" t="s">
+      <c r="O46" s="60"/>
+      <c r="P46" s="60"/>
+      <c r="Q46" s="60"/>
+      <c r="R46" s="60"/>
+      <c r="S46" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="T46" s="62"/>
-      <c r="U46" s="62"/>
-      <c r="V46" s="62"/>
-      <c r="W46" s="62"/>
-      <c r="X46" s="62"/>
-      <c r="Y46" s="62"/>
+      <c r="T46" s="60"/>
+      <c r="U46" s="60"/>
+      <c r="V46" s="60"/>
+      <c r="W46" s="60"/>
+      <c r="X46" s="60"/>
+      <c r="Y46" s="60"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H47" s="37"/>
@@ -2897,22 +2897,22 @@
       <c r="J47" s="31"/>
       <c r="K47" s="38"/>
       <c r="L47" s="37"/>
-      <c r="N47" s="62" t="s">
+      <c r="N47" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="O47" s="62"/>
-      <c r="P47" s="62"/>
-      <c r="Q47" s="62"/>
-      <c r="R47" s="62"/>
-      <c r="S47" s="62" t="s">
+      <c r="O47" s="60"/>
+      <c r="P47" s="60"/>
+      <c r="Q47" s="60"/>
+      <c r="R47" s="60"/>
+      <c r="S47" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="T47" s="62"/>
-      <c r="U47" s="62"/>
-      <c r="V47" s="62"/>
-      <c r="W47" s="62"/>
-      <c r="X47" s="62"/>
-      <c r="Y47" s="62"/>
+      <c r="T47" s="60"/>
+      <c r="U47" s="60"/>
+      <c r="V47" s="60"/>
+      <c r="W47" s="60"/>
+      <c r="X47" s="60"/>
+      <c r="Y47" s="60"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H48" s="32"/>
@@ -2920,20 +2920,20 @@
       <c r="J48" s="38"/>
       <c r="K48" s="37"/>
       <c r="L48" s="32"/>
-      <c r="N48" s="62"/>
-      <c r="O48" s="62"/>
-      <c r="P48" s="62"/>
-      <c r="Q48" s="62"/>
-      <c r="R48" s="62"/>
-      <c r="S48" s="62" t="s">
+      <c r="N48" s="60"/>
+      <c r="O48" s="60"/>
+      <c r="P48" s="60"/>
+      <c r="Q48" s="60"/>
+      <c r="R48" s="60"/>
+      <c r="S48" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="T48" s="62"/>
-      <c r="U48" s="62"/>
-      <c r="V48" s="62"/>
-      <c r="W48" s="62"/>
-      <c r="X48" s="62"/>
-      <c r="Y48" s="62"/>
+      <c r="T48" s="60"/>
+      <c r="U48" s="60"/>
+      <c r="V48" s="60"/>
+      <c r="W48" s="60"/>
+      <c r="X48" s="60"/>
+      <c r="Y48" s="60"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H49" s="37"/>
@@ -2941,42 +2941,42 @@
       <c r="J49" s="37"/>
       <c r="K49" s="32"/>
       <c r="L49" s="37"/>
-      <c r="N49" s="62"/>
-      <c r="O49" s="62"/>
-      <c r="P49" s="62"/>
-      <c r="Q49" s="62"/>
-      <c r="R49" s="62"/>
-      <c r="S49" s="62" t="s">
+      <c r="N49" s="60"/>
+      <c r="O49" s="60"/>
+      <c r="P49" s="60"/>
+      <c r="Q49" s="60"/>
+      <c r="R49" s="60"/>
+      <c r="S49" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="T49" s="62"/>
-      <c r="U49" s="62"/>
-      <c r="V49" s="62"/>
-      <c r="W49" s="62"/>
-      <c r="X49" s="62"/>
-      <c r="Y49" s="62"/>
+      <c r="T49" s="60"/>
+      <c r="U49" s="60"/>
+      <c r="V49" s="60"/>
+      <c r="W49" s="60"/>
+      <c r="X49" s="60"/>
+      <c r="Y49" s="60"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N50" s="60"/>
-      <c r="O50" s="60"/>
-      <c r="P50" s="60"/>
-      <c r="Q50" s="60"/>
-      <c r="R50" s="60"/>
-      <c r="S50" s="60" t="s">
+      <c r="N50" s="62"/>
+      <c r="O50" s="62"/>
+      <c r="P50" s="62"/>
+      <c r="Q50" s="62"/>
+      <c r="R50" s="62"/>
+      <c r="S50" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="T50" s="60"/>
-      <c r="U50" s="60"/>
-      <c r="V50" s="60"/>
-      <c r="W50" s="60"/>
-      <c r="X50" s="60"/>
-      <c r="Y50" s="60"/>
+      <c r="T50" s="62"/>
+      <c r="U50" s="62"/>
+      <c r="V50" s="62"/>
+      <c r="W50" s="62"/>
+      <c r="X50" s="62"/>
+      <c r="Y50" s="62"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A52" s="61" t="s">
+      <c r="A52" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="61"/>
+      <c r="B52" s="67"/>
     </row>
     <row r="54" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
@@ -2994,13 +2994,13 @@
       <c r="E54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="68" t="s">
+      <c r="H54" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I54" s="68"/>
-      <c r="J54" s="68"/>
-      <c r="K54" s="68"/>
-      <c r="L54" s="68"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="63"/>
       <c r="M54" s="33"/>
       <c r="N54" s="33"/>
     </row>
@@ -3012,13 +3012,13 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="H55" s="65" t="s">
+      <c r="H55" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="I55" s="65"/>
-      <c r="J55" s="65"/>
-      <c r="K55" s="65"/>
-      <c r="L55" s="65"/>
+      <c r="I55" s="64"/>
+      <c r="J55" s="64"/>
+      <c r="K55" s="64"/>
+      <c r="L55" s="64"/>
       <c r="M55" t="s">
         <v>70</v>
       </c>
@@ -3031,14 +3031,14 @@
       <c r="P55" t="s">
         <v>67</v>
       </c>
-      <c r="T55" s="68" t="s">
+      <c r="T55" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="U55" s="68"/>
-      <c r="V55" s="68" t="s">
+      <c r="U55" s="63"/>
+      <c r="V55" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="W55" s="68"/>
+      <c r="W55" s="63"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
@@ -3056,31 +3056,31 @@
       <c r="E56" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="65" t="s">
+      <c r="H56" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="I56" s="65"/>
-      <c r="J56" s="65"/>
-      <c r="K56" s="65"/>
-      <c r="L56" s="65"/>
-      <c r="M56" s="66" t="s">
+      <c r="I56" s="64"/>
+      <c r="J56" s="64"/>
+      <c r="K56" s="64"/>
+      <c r="L56" s="64"/>
+      <c r="M56" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="N56" s="66"/>
+      <c r="N56" s="61"/>
       <c r="O56" t="s">
         <v>72</v>
       </c>
       <c r="S56" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="T56" s="61" t="s">
+      <c r="T56" s="67" t="s">
         <v>111</v>
       </c>
-      <c r="U56" s="61"/>
-      <c r="V56" s="61" t="s">
+      <c r="U56" s="67"/>
+      <c r="V56" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="W56" s="61"/>
+      <c r="W56" s="67"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
@@ -3098,34 +3098,34 @@
       <c r="E57" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H57" s="65" t="s">
+      <c r="H57" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="I57" s="65"/>
-      <c r="J57" s="65"/>
-      <c r="K57" s="65"/>
-      <c r="L57" s="65"/>
-      <c r="M57" s="66" t="s">
+      <c r="I57" s="64"/>
+      <c r="J57" s="64"/>
+      <c r="K57" s="64"/>
+      <c r="L57" s="64"/>
+      <c r="M57" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="N57" s="66"/>
-      <c r="O57" s="66" t="s">
+      <c r="N57" s="61"/>
+      <c r="O57" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="P57" s="66"/>
+      <c r="P57" s="61"/>
       <c r="Q57" s="33"/>
       <c r="R57" s="33"/>
       <c r="S57" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="T57" s="61" t="s">
+      <c r="T57" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="U57" s="61"/>
-      <c r="V57" s="61" t="s">
+      <c r="U57" s="67"/>
+      <c r="V57" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="W57" s="61"/>
+      <c r="W57" s="67"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
@@ -3143,13 +3143,13 @@
       <c r="E58" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H58" s="67" t="s">
+      <c r="H58" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="I58" s="67"/>
-      <c r="J58" s="67"/>
-      <c r="K58" s="67"/>
-      <c r="L58" s="67"/>
+      <c r="I58" s="68"/>
+      <c r="J58" s="68"/>
+      <c r="K58" s="68"/>
+      <c r="L58" s="68"/>
       <c r="M58" s="43" t="s">
         <v>64</v>
       </c>
@@ -3182,10 +3182,10 @@
       <c r="N59" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S59" s="68" t="s">
+      <c r="S59" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T59" s="68"/>
+      <c r="T59" s="63"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -3200,22 +3200,22 @@
       <c r="J60" s="37"/>
       <c r="K60" s="32"/>
       <c r="L60" s="37"/>
-      <c r="N60" s="62" t="s">
+      <c r="N60" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="O60" s="62"/>
-      <c r="P60" s="62"/>
-      <c r="Q60" s="62"/>
-      <c r="R60" s="62"/>
-      <c r="S60" s="62" t="s">
+      <c r="O60" s="60"/>
+      <c r="P60" s="60"/>
+      <c r="Q60" s="60"/>
+      <c r="R60" s="60"/>
+      <c r="S60" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="T60" s="62"/>
-      <c r="U60" s="62"/>
-      <c r="V60" s="62"/>
-      <c r="W60" s="62"/>
-      <c r="X60" s="62"/>
-      <c r="Y60" s="62"/>
+      <c r="T60" s="60"/>
+      <c r="U60" s="60"/>
+      <c r="V60" s="60"/>
+      <c r="W60" s="60"/>
+      <c r="X60" s="60"/>
+      <c r="Y60" s="60"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
@@ -3238,22 +3238,22 @@
       <c r="J61" s="31"/>
       <c r="K61" s="37"/>
       <c r="L61" s="32"/>
-      <c r="N61" s="62" t="s">
+      <c r="N61" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="O61" s="62"/>
-      <c r="P61" s="62"/>
-      <c r="Q61" s="62"/>
-      <c r="R61" s="62"/>
-      <c r="S61" s="62" t="s">
+      <c r="O61" s="60"/>
+      <c r="P61" s="60"/>
+      <c r="Q61" s="60"/>
+      <c r="R61" s="60"/>
+      <c r="S61" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="T61" s="62"/>
-      <c r="U61" s="62"/>
-      <c r="V61" s="62"/>
-      <c r="W61" s="62"/>
-      <c r="X61" s="62"/>
-      <c r="Y61" s="62"/>
+      <c r="T61" s="60"/>
+      <c r="U61" s="60"/>
+      <c r="V61" s="60"/>
+      <c r="W61" s="60"/>
+      <c r="X61" s="60"/>
+      <c r="Y61" s="60"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
@@ -3276,22 +3276,22 @@
       <c r="J62" s="31"/>
       <c r="K62" s="38"/>
       <c r="L62" s="37"/>
-      <c r="N62" s="62" t="s">
+      <c r="N62" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="O62" s="62"/>
-      <c r="P62" s="62"/>
-      <c r="Q62" s="62"/>
-      <c r="R62" s="62"/>
-      <c r="S62" s="62" t="s">
+      <c r="O62" s="60"/>
+      <c r="P62" s="60"/>
+      <c r="Q62" s="60"/>
+      <c r="R62" s="60"/>
+      <c r="S62" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="T62" s="62"/>
-      <c r="U62" s="62"/>
-      <c r="V62" s="62"/>
-      <c r="W62" s="62"/>
-      <c r="X62" s="62"/>
-      <c r="Y62" s="62"/>
+      <c r="T62" s="60"/>
+      <c r="U62" s="60"/>
+      <c r="V62" s="60"/>
+      <c r="W62" s="60"/>
+      <c r="X62" s="60"/>
+      <c r="Y62" s="60"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H63" s="32"/>
@@ -3299,22 +3299,22 @@
       <c r="J63" s="38"/>
       <c r="K63" s="37"/>
       <c r="L63" s="32"/>
-      <c r="N63" s="62" t="s">
+      <c r="N63" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="O63" s="62"/>
-      <c r="P63" s="62"/>
-      <c r="Q63" s="62"/>
-      <c r="R63" s="62"/>
-      <c r="S63" s="62" t="s">
+      <c r="O63" s="60"/>
+      <c r="P63" s="60"/>
+      <c r="Q63" s="60"/>
+      <c r="R63" s="60"/>
+      <c r="S63" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="T63" s="62"/>
-      <c r="U63" s="62"/>
-      <c r="V63" s="62"/>
-      <c r="W63" s="62"/>
-      <c r="X63" s="62"/>
-      <c r="Y63" s="62"/>
+      <c r="T63" s="60"/>
+      <c r="U63" s="60"/>
+      <c r="V63" s="60"/>
+      <c r="W63" s="60"/>
+      <c r="X63" s="60"/>
+      <c r="Y63" s="60"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H64" s="37"/>
@@ -3322,38 +3322,38 @@
       <c r="J64" s="37"/>
       <c r="K64" s="32"/>
       <c r="L64" s="37"/>
-      <c r="N64" s="62" t="s">
+      <c r="N64" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="O64" s="62"/>
-      <c r="P64" s="62"/>
-      <c r="Q64" s="62"/>
-      <c r="R64" s="62"/>
-      <c r="S64" s="62" t="s">
+      <c r="O64" s="60"/>
+      <c r="P64" s="60"/>
+      <c r="Q64" s="60"/>
+      <c r="R64" s="60"/>
+      <c r="S64" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="T64" s="62"/>
-      <c r="U64" s="62"/>
-      <c r="V64" s="62"/>
-      <c r="W64" s="62"/>
-      <c r="X64" s="62"/>
-      <c r="Y64" s="62"/>
+      <c r="T64" s="60"/>
+      <c r="U64" s="60"/>
+      <c r="V64" s="60"/>
+      <c r="W64" s="60"/>
+      <c r="X64" s="60"/>
+      <c r="Y64" s="60"/>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N65" s="60"/>
-      <c r="O65" s="60"/>
-      <c r="P65" s="60"/>
-      <c r="Q65" s="60"/>
-      <c r="R65" s="60"/>
-      <c r="S65" s="60" t="s">
+      <c r="N65" s="62"/>
+      <c r="O65" s="62"/>
+      <c r="P65" s="62"/>
+      <c r="Q65" s="62"/>
+      <c r="R65" s="62"/>
+      <c r="S65" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="T65" s="60"/>
-      <c r="U65" s="60"/>
-      <c r="V65" s="60"/>
-      <c r="W65" s="60"/>
-      <c r="X65" s="60"/>
-      <c r="Y65" s="60"/>
+      <c r="T65" s="62"/>
+      <c r="U65" s="62"/>
+      <c r="V65" s="62"/>
+      <c r="W65" s="62"/>
+      <c r="X65" s="62"/>
+      <c r="Y65" s="62"/>
     </row>
     <row r="67" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="26" t="s">
@@ -3371,13 +3371,13 @@
       <c r="E67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="68" t="s">
+      <c r="H67" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I67" s="68"/>
-      <c r="J67" s="68"/>
-      <c r="K67" s="68"/>
-      <c r="L67" s="68"/>
+      <c r="I67" s="63"/>
+      <c r="J67" s="63"/>
+      <c r="K67" s="63"/>
+      <c r="L67" s="63"/>
       <c r="M67" s="33"/>
       <c r="N67" s="33"/>
     </row>
@@ -3389,13 +3389,13 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="H68" s="65" t="s">
+      <c r="H68" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="I68" s="65"/>
-      <c r="J68" s="65"/>
-      <c r="K68" s="65"/>
-      <c r="L68" s="65"/>
+      <c r="I68" s="64"/>
+      <c r="J68" s="64"/>
+      <c r="K68" s="64"/>
+      <c r="L68" s="64"/>
       <c r="M68" t="s">
         <v>70</v>
       </c>
@@ -3408,14 +3408,14 @@
       <c r="P68" t="s">
         <v>67</v>
       </c>
-      <c r="T68" s="68" t="s">
+      <c r="T68" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="U68" s="68"/>
-      <c r="V68" s="68" t="s">
+      <c r="U68" s="63"/>
+      <c r="V68" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="W68" s="68"/>
+      <c r="W68" s="63"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
@@ -3433,31 +3433,31 @@
       <c r="E69" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H69" s="63" t="s">
+      <c r="H69" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="I69" s="63"/>
-      <c r="J69" s="63"/>
-      <c r="K69" s="63"/>
-      <c r="L69" s="63"/>
-      <c r="M69" s="64" t="s">
+      <c r="I69" s="65"/>
+      <c r="J69" s="65"/>
+      <c r="K69" s="65"/>
+      <c r="L69" s="65"/>
+      <c r="M69" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="N69" s="64"/>
+      <c r="N69" s="66"/>
       <c r="O69" t="s">
         <v>72</v>
       </c>
       <c r="S69" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="T69" s="61" t="s">
+      <c r="T69" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="U69" s="61"/>
-      <c r="V69" s="61" t="s">
+      <c r="U69" s="67"/>
+      <c r="V69" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="W69" s="61"/>
+      <c r="W69" s="67"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
@@ -3475,21 +3475,21 @@
       <c r="E70" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H70" s="65" t="s">
+      <c r="H70" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="I70" s="65"/>
-      <c r="J70" s="65"/>
-      <c r="K70" s="65"/>
-      <c r="L70" s="65"/>
-      <c r="M70" s="66" t="s">
+      <c r="I70" s="64"/>
+      <c r="J70" s="64"/>
+      <c r="K70" s="64"/>
+      <c r="L70" s="64"/>
+      <c r="M70" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="N70" s="66"/>
-      <c r="O70" s="66" t="s">
+      <c r="N70" s="61"/>
+      <c r="O70" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="P70" s="66"/>
+      <c r="P70" s="61"/>
       <c r="Q70" s="33"/>
       <c r="R70" s="33"/>
     </row>
@@ -3509,13 +3509,13 @@
       <c r="E71" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H71" s="67" t="s">
+      <c r="H71" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="I71" s="67"/>
-      <c r="J71" s="67"/>
-      <c r="K71" s="67"/>
-      <c r="L71" s="67"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="68"/>
+      <c r="K71" s="68"/>
+      <c r="L71" s="68"/>
       <c r="M71" s="43" t="s">
         <v>64</v>
       </c>
@@ -3548,10 +3548,10 @@
       <c r="N72" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S72" s="68" t="s">
+      <c r="S72" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T72" s="68"/>
+      <c r="T72" s="63"/>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -3566,22 +3566,22 @@
       <c r="J73" s="37"/>
       <c r="K73" s="32"/>
       <c r="L73" s="37"/>
-      <c r="N73" s="62" t="s">
+      <c r="N73" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="O73" s="62"/>
-      <c r="P73" s="62"/>
-      <c r="Q73" s="62"/>
-      <c r="R73" s="62"/>
-      <c r="S73" s="62" t="s">
+      <c r="O73" s="60"/>
+      <c r="P73" s="60"/>
+      <c r="Q73" s="60"/>
+      <c r="R73" s="60"/>
+      <c r="S73" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="T73" s="62"/>
-      <c r="U73" s="62"/>
-      <c r="V73" s="62"/>
-      <c r="W73" s="62"/>
-      <c r="X73" s="62"/>
-      <c r="Y73" s="62"/>
+      <c r="T73" s="60"/>
+      <c r="U73" s="60"/>
+      <c r="V73" s="60"/>
+      <c r="W73" s="60"/>
+      <c r="X73" s="60"/>
+      <c r="Y73" s="60"/>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
@@ -3604,20 +3604,20 @@
       <c r="J74" s="31"/>
       <c r="K74" s="37"/>
       <c r="L74" s="32"/>
-      <c r="N74" s="62" t="s">
+      <c r="N74" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="O74" s="62"/>
-      <c r="P74" s="62"/>
-      <c r="Q74" s="62"/>
-      <c r="R74" s="62"/>
-      <c r="S74" s="62"/>
-      <c r="T74" s="62"/>
-      <c r="U74" s="62"/>
-      <c r="V74" s="62"/>
-      <c r="W74" s="62"/>
-      <c r="X74" s="62"/>
-      <c r="Y74" s="62"/>
+      <c r="O74" s="60"/>
+      <c r="P74" s="60"/>
+      <c r="Q74" s="60"/>
+      <c r="R74" s="60"/>
+      <c r="S74" s="60"/>
+      <c r="T74" s="60"/>
+      <c r="U74" s="60"/>
+      <c r="V74" s="60"/>
+      <c r="W74" s="60"/>
+      <c r="X74" s="60"/>
+      <c r="Y74" s="60"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
@@ -3640,18 +3640,18 @@
       <c r="J75" s="31"/>
       <c r="K75" s="38"/>
       <c r="L75" s="37"/>
-      <c r="N75" s="62"/>
-      <c r="O75" s="62"/>
-      <c r="P75" s="62"/>
-      <c r="Q75" s="62"/>
-      <c r="R75" s="62"/>
-      <c r="S75" s="62"/>
-      <c r="T75" s="62"/>
-      <c r="U75" s="62"/>
-      <c r="V75" s="62"/>
-      <c r="W75" s="62"/>
-      <c r="X75" s="62"/>
-      <c r="Y75" s="62"/>
+      <c r="N75" s="60"/>
+      <c r="O75" s="60"/>
+      <c r="P75" s="60"/>
+      <c r="Q75" s="60"/>
+      <c r="R75" s="60"/>
+      <c r="S75" s="60"/>
+      <c r="T75" s="60"/>
+      <c r="U75" s="60"/>
+      <c r="V75" s="60"/>
+      <c r="W75" s="60"/>
+      <c r="X75" s="60"/>
+      <c r="Y75" s="60"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H76" s="32"/>
@@ -3659,18 +3659,18 @@
       <c r="J76" s="38"/>
       <c r="K76" s="37"/>
       <c r="L76" s="32"/>
-      <c r="N76" s="62"/>
-      <c r="O76" s="62"/>
-      <c r="P76" s="62"/>
-      <c r="Q76" s="62"/>
-      <c r="R76" s="62"/>
-      <c r="S76" s="62"/>
-      <c r="T76" s="62"/>
-      <c r="U76" s="62"/>
-      <c r="V76" s="62"/>
-      <c r="W76" s="62"/>
-      <c r="X76" s="62"/>
-      <c r="Y76" s="62"/>
+      <c r="N76" s="60"/>
+      <c r="O76" s="60"/>
+      <c r="P76" s="60"/>
+      <c r="Q76" s="60"/>
+      <c r="R76" s="60"/>
+      <c r="S76" s="60"/>
+      <c r="T76" s="60"/>
+      <c r="U76" s="60"/>
+      <c r="V76" s="60"/>
+      <c r="W76" s="60"/>
+      <c r="X76" s="60"/>
+      <c r="Y76" s="60"/>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H77" s="37"/>
@@ -3678,36 +3678,36 @@
       <c r="J77" s="37"/>
       <c r="K77" s="32"/>
       <c r="L77" s="37"/>
-      <c r="N77" s="62"/>
-      <c r="O77" s="62"/>
-      <c r="P77" s="62"/>
-      <c r="Q77" s="62"/>
-      <c r="R77" s="62"/>
-      <c r="S77" s="62"/>
-      <c r="T77" s="62"/>
-      <c r="U77" s="62"/>
-      <c r="V77" s="62"/>
-      <c r="W77" s="62"/>
-      <c r="X77" s="62"/>
-      <c r="Y77" s="62"/>
+      <c r="N77" s="60"/>
+      <c r="O77" s="60"/>
+      <c r="P77" s="60"/>
+      <c r="Q77" s="60"/>
+      <c r="R77" s="60"/>
+      <c r="S77" s="60"/>
+      <c r="T77" s="60"/>
+      <c r="U77" s="60"/>
+      <c r="V77" s="60"/>
+      <c r="W77" s="60"/>
+      <c r="X77" s="60"/>
+      <c r="Y77" s="60"/>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A78" s="61" t="s">
+      <c r="A78" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="B78" s="61"/>
-      <c r="N78" s="60"/>
-      <c r="O78" s="60"/>
-      <c r="P78" s="60"/>
-      <c r="Q78" s="60"/>
-      <c r="R78" s="60"/>
-      <c r="S78" s="60"/>
-      <c r="T78" s="60"/>
-      <c r="U78" s="60"/>
-      <c r="V78" s="60"/>
-      <c r="W78" s="60"/>
-      <c r="X78" s="60"/>
-      <c r="Y78" s="60"/>
+      <c r="B78" s="67"/>
+      <c r="N78" s="62"/>
+      <c r="O78" s="62"/>
+      <c r="P78" s="62"/>
+      <c r="Q78" s="62"/>
+      <c r="R78" s="62"/>
+      <c r="S78" s="62"/>
+      <c r="T78" s="62"/>
+      <c r="U78" s="62"/>
+      <c r="V78" s="62"/>
+      <c r="W78" s="62"/>
+      <c r="X78" s="62"/>
+      <c r="Y78" s="62"/>
     </row>
     <row r="80" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="26" t="s">
@@ -3725,13 +3725,13 @@
       <c r="E80" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H80" s="68" t="s">
+      <c r="H80" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I80" s="68"/>
-      <c r="J80" s="68"/>
-      <c r="K80" s="68"/>
-      <c r="L80" s="68"/>
+      <c r="I80" s="63"/>
+      <c r="J80" s="63"/>
+      <c r="K80" s="63"/>
+      <c r="L80" s="63"/>
       <c r="M80" s="33"/>
       <c r="N80" s="33"/>
     </row>
@@ -3743,13 +3743,13 @@
       <c r="C81" s="25"/>
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
-      <c r="H81" s="65" t="s">
+      <c r="H81" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="I81" s="65"/>
-      <c r="J81" s="65"/>
-      <c r="K81" s="65"/>
-      <c r="L81" s="65"/>
+      <c r="I81" s="64"/>
+      <c r="J81" s="64"/>
+      <c r="K81" s="64"/>
+      <c r="L81" s="64"/>
       <c r="M81" t="s">
         <v>70</v>
       </c>
@@ -3762,14 +3762,14 @@
       <c r="P81" t="s">
         <v>67</v>
       </c>
-      <c r="T81" s="68" t="s">
+      <c r="T81" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="U81" s="68"/>
-      <c r="V81" s="68" t="s">
+      <c r="U81" s="63"/>
+      <c r="V81" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="W81" s="68"/>
+      <c r="W81" s="63"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
@@ -3787,17 +3787,17 @@
       <c r="E82" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H82" s="63" t="s">
+      <c r="H82" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="I82" s="63"/>
-      <c r="J82" s="63"/>
-      <c r="K82" s="63"/>
-      <c r="L82" s="63"/>
-      <c r="M82" s="64" t="s">
+      <c r="I82" s="65"/>
+      <c r="J82" s="65"/>
+      <c r="K82" s="65"/>
+      <c r="L82" s="65"/>
+      <c r="M82" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="N82" s="64"/>
+      <c r="N82" s="66"/>
       <c r="O82" t="s">
         <v>72</v>
       </c>
@@ -3807,14 +3807,14 @@
       <c r="S82" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="T82" s="61" t="s">
+      <c r="T82" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="U82" s="61"/>
-      <c r="V82" s="61" t="s">
+      <c r="U82" s="67"/>
+      <c r="V82" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="W82" s="61"/>
+      <c r="W82" s="67"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
@@ -3832,21 +3832,21 @@
       <c r="E83" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H83" s="65" t="s">
+      <c r="H83" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
-      <c r="K83" s="65"/>
-      <c r="L83" s="65"/>
-      <c r="M83" s="66" t="s">
+      <c r="I83" s="64"/>
+      <c r="J83" s="64"/>
+      <c r="K83" s="64"/>
+      <c r="L83" s="64"/>
+      <c r="M83" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="N83" s="66"/>
-      <c r="O83" s="66" t="s">
+      <c r="N83" s="61"/>
+      <c r="O83" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="P83" s="66"/>
+      <c r="P83" s="61"/>
       <c r="Q83" s="33"/>
       <c r="R83" s="33"/>
     </row>
@@ -3866,13 +3866,13 @@
       <c r="E84" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H84" s="67" t="s">
+      <c r="H84" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="I84" s="67"/>
-      <c r="J84" s="67"/>
-      <c r="K84" s="67"/>
-      <c r="L84" s="67"/>
+      <c r="I84" s="68"/>
+      <c r="J84" s="68"/>
+      <c r="K84" s="68"/>
+      <c r="L84" s="68"/>
       <c r="M84" s="43" t="s">
         <v>64</v>
       </c>
@@ -3905,10 +3905,10 @@
       <c r="N85" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S85" s="68" t="s">
+      <c r="S85" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T85" s="68"/>
+      <c r="T85" s="63"/>
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" s="34" t="s">
@@ -3923,22 +3923,22 @@
       <c r="J86" s="37"/>
       <c r="K86" s="32"/>
       <c r="L86" s="37"/>
-      <c r="N86" s="62" t="s">
+      <c r="N86" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="O86" s="62"/>
-      <c r="P86" s="62"/>
-      <c r="Q86" s="62"/>
-      <c r="R86" s="62"/>
-      <c r="S86" s="62" t="s">
+      <c r="O86" s="60"/>
+      <c r="P86" s="60"/>
+      <c r="Q86" s="60"/>
+      <c r="R86" s="60"/>
+      <c r="S86" s="60" t="s">
         <v>130</v>
       </c>
-      <c r="T86" s="62"/>
-      <c r="U86" s="62"/>
-      <c r="V86" s="62"/>
-      <c r="W86" s="62"/>
-      <c r="X86" s="62"/>
-      <c r="Y86" s="62"/>
+      <c r="T86" s="60"/>
+      <c r="U86" s="60"/>
+      <c r="V86" s="60"/>
+      <c r="W86" s="60"/>
+      <c r="X86" s="60"/>
+      <c r="Y86" s="60"/>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
@@ -3961,22 +3961,22 @@
       <c r="J87" s="31"/>
       <c r="K87" s="37"/>
       <c r="L87" s="32"/>
-      <c r="N87" s="62" t="s">
+      <c r="N87" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="O87" s="62"/>
-      <c r="P87" s="62"/>
-      <c r="Q87" s="62"/>
-      <c r="R87" s="62"/>
-      <c r="S87" s="62" t="s">
+      <c r="O87" s="60"/>
+      <c r="P87" s="60"/>
+      <c r="Q87" s="60"/>
+      <c r="R87" s="60"/>
+      <c r="S87" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="T87" s="62"/>
-      <c r="U87" s="62"/>
-      <c r="V87" s="62"/>
-      <c r="W87" s="62"/>
-      <c r="X87" s="62"/>
-      <c r="Y87" s="62"/>
+      <c r="T87" s="60"/>
+      <c r="U87" s="60"/>
+      <c r="V87" s="60"/>
+      <c r="W87" s="60"/>
+      <c r="X87" s="60"/>
+      <c r="Y87" s="60"/>
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
@@ -3999,22 +3999,22 @@
       <c r="J88" s="31"/>
       <c r="K88" s="38"/>
       <c r="L88" s="37"/>
-      <c r="N88" s="62" t="s">
+      <c r="N88" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="O88" s="62"/>
-      <c r="P88" s="62"/>
-      <c r="Q88" s="62"/>
-      <c r="R88" s="62"/>
-      <c r="S88" s="62" t="s">
+      <c r="O88" s="60"/>
+      <c r="P88" s="60"/>
+      <c r="Q88" s="60"/>
+      <c r="R88" s="60"/>
+      <c r="S88" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="T88" s="62"/>
-      <c r="U88" s="62"/>
-      <c r="V88" s="62"/>
-      <c r="W88" s="62"/>
-      <c r="X88" s="62"/>
-      <c r="Y88" s="62"/>
+      <c r="T88" s="60"/>
+      <c r="U88" s="60"/>
+      <c r="V88" s="60"/>
+      <c r="W88" s="60"/>
+      <c r="X88" s="60"/>
+      <c r="Y88" s="60"/>
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H89" s="32"/>
@@ -4022,20 +4022,20 @@
       <c r="J89" s="38"/>
       <c r="K89" s="37"/>
       <c r="L89" s="32"/>
-      <c r="N89" s="62"/>
-      <c r="O89" s="62"/>
-      <c r="P89" s="62"/>
-      <c r="Q89" s="62"/>
-      <c r="R89" s="62"/>
-      <c r="S89" s="62" t="s">
+      <c r="N89" s="60"/>
+      <c r="O89" s="60"/>
+      <c r="P89" s="60"/>
+      <c r="Q89" s="60"/>
+      <c r="R89" s="60"/>
+      <c r="S89" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="T89" s="62"/>
-      <c r="U89" s="62"/>
-      <c r="V89" s="62"/>
-      <c r="W89" s="62"/>
-      <c r="X89" s="62"/>
-      <c r="Y89" s="62"/>
+      <c r="T89" s="60"/>
+      <c r="U89" s="60"/>
+      <c r="V89" s="60"/>
+      <c r="W89" s="60"/>
+      <c r="X89" s="60"/>
+      <c r="Y89" s="60"/>
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H90" s="37"/>
@@ -4043,110 +4043,94 @@
       <c r="J90" s="37"/>
       <c r="K90" s="32"/>
       <c r="L90" s="37"/>
-      <c r="N90" s="62"/>
-      <c r="O90" s="62"/>
-      <c r="P90" s="62"/>
-      <c r="Q90" s="62"/>
-      <c r="R90" s="62"/>
-      <c r="S90" s="62" t="s">
+      <c r="N90" s="60"/>
+      <c r="O90" s="60"/>
+      <c r="P90" s="60"/>
+      <c r="Q90" s="60"/>
+      <c r="R90" s="60"/>
+      <c r="S90" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="T90" s="62"/>
-      <c r="U90" s="62"/>
-      <c r="V90" s="62"/>
-      <c r="W90" s="62"/>
-      <c r="X90" s="62"/>
-      <c r="Y90" s="62"/>
+      <c r="T90" s="60"/>
+      <c r="U90" s="60"/>
+      <c r="V90" s="60"/>
+      <c r="W90" s="60"/>
+      <c r="X90" s="60"/>
+      <c r="Y90" s="60"/>
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N91" s="60"/>
-      <c r="O91" s="60"/>
-      <c r="P91" s="60"/>
-      <c r="Q91" s="60"/>
-      <c r="R91" s="60"/>
-      <c r="S91" s="60"/>
-      <c r="T91" s="60"/>
-      <c r="U91" s="60"/>
-      <c r="V91" s="60"/>
-      <c r="W91" s="60"/>
-      <c r="X91" s="60"/>
-      <c r="Y91" s="60"/>
+      <c r="N91" s="62"/>
+      <c r="O91" s="62"/>
+      <c r="P91" s="62"/>
+      <c r="Q91" s="62"/>
+      <c r="R91" s="62"/>
+      <c r="S91" s="62"/>
+      <c r="T91" s="62"/>
+      <c r="U91" s="62"/>
+      <c r="V91" s="62"/>
+      <c r="W91" s="62"/>
+      <c r="X91" s="62"/>
+      <c r="Y91" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="154">
-    <mergeCell ref="N75:R75"/>
-    <mergeCell ref="S75:Y75"/>
-    <mergeCell ref="N76:R76"/>
-    <mergeCell ref="S76:Y76"/>
-    <mergeCell ref="N77:R77"/>
-    <mergeCell ref="S77:Y77"/>
-    <mergeCell ref="O70:P70"/>
-    <mergeCell ref="N64:R64"/>
-    <mergeCell ref="S64:Y64"/>
-    <mergeCell ref="N65:R65"/>
-    <mergeCell ref="S65:Y65"/>
-    <mergeCell ref="N74:R74"/>
-    <mergeCell ref="S74:Y74"/>
-    <mergeCell ref="H67:L67"/>
-    <mergeCell ref="H68:L68"/>
-    <mergeCell ref="H69:L69"/>
-    <mergeCell ref="M69:N69"/>
-    <mergeCell ref="H70:L70"/>
-    <mergeCell ref="M70:N70"/>
-    <mergeCell ref="T69:U69"/>
-    <mergeCell ref="V69:W69"/>
-    <mergeCell ref="T68:U68"/>
-    <mergeCell ref="V68:W68"/>
-    <mergeCell ref="N61:R61"/>
-    <mergeCell ref="S61:Y61"/>
-    <mergeCell ref="N62:R62"/>
-    <mergeCell ref="S62:Y62"/>
-    <mergeCell ref="N63:R63"/>
-    <mergeCell ref="S63:Y63"/>
-    <mergeCell ref="H71:L71"/>
-    <mergeCell ref="S72:T72"/>
-    <mergeCell ref="N73:R73"/>
-    <mergeCell ref="S73:Y73"/>
-    <mergeCell ref="H55:L55"/>
-    <mergeCell ref="H56:L56"/>
-    <mergeCell ref="M56:N56"/>
-    <mergeCell ref="H58:L58"/>
-    <mergeCell ref="S59:T59"/>
-    <mergeCell ref="N60:R60"/>
-    <mergeCell ref="S60:Y60"/>
-    <mergeCell ref="S48:Y48"/>
-    <mergeCell ref="S49:Y49"/>
-    <mergeCell ref="S50:Y50"/>
-    <mergeCell ref="N50:R50"/>
-    <mergeCell ref="H57:L57"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="T55:U55"/>
-    <mergeCell ref="T56:U56"/>
-    <mergeCell ref="V55:W55"/>
-    <mergeCell ref="V56:W56"/>
-    <mergeCell ref="V57:W57"/>
-    <mergeCell ref="T57:U57"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="H54:L54"/>
-    <mergeCell ref="S36:Y36"/>
-    <mergeCell ref="S37:Y37"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="S45:Y45"/>
-    <mergeCell ref="S46:Y46"/>
-    <mergeCell ref="S47:Y47"/>
-    <mergeCell ref="S24:Y24"/>
-    <mergeCell ref="S25:Y25"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="S33:Y33"/>
-    <mergeCell ref="S34:Y34"/>
-    <mergeCell ref="S35:Y35"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="N91:R91"/>
+    <mergeCell ref="S91:Y91"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="N86:R86"/>
+    <mergeCell ref="S86:Y86"/>
+    <mergeCell ref="N87:R87"/>
+    <mergeCell ref="S87:Y87"/>
+    <mergeCell ref="N88:R88"/>
+    <mergeCell ref="S88:Y88"/>
+    <mergeCell ref="N89:R89"/>
+    <mergeCell ref="S89:Y89"/>
+    <mergeCell ref="N90:R90"/>
+    <mergeCell ref="S90:Y90"/>
+    <mergeCell ref="H82:L82"/>
+    <mergeCell ref="M82:N82"/>
+    <mergeCell ref="T82:U82"/>
+    <mergeCell ref="V82:W82"/>
+    <mergeCell ref="H83:L83"/>
+    <mergeCell ref="M83:N83"/>
+    <mergeCell ref="O83:P83"/>
+    <mergeCell ref="H84:L84"/>
+    <mergeCell ref="S85:T85"/>
+    <mergeCell ref="N78:R78"/>
+    <mergeCell ref="S78:Y78"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="H80:L80"/>
+    <mergeCell ref="H81:L81"/>
+    <mergeCell ref="T81:U81"/>
+    <mergeCell ref="V81:W81"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="N22:R22"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="N25:R25"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="N10:R10"/>
     <mergeCell ref="S9:Y9"/>
     <mergeCell ref="S10:Y10"/>
     <mergeCell ref="S11:Y11"/>
@@ -4171,63 +4155,79 @@
     <mergeCell ref="N34:R34"/>
     <mergeCell ref="N11:R11"/>
     <mergeCell ref="N12:R12"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="H80:L80"/>
-    <mergeCell ref="H81:L81"/>
-    <mergeCell ref="T81:U81"/>
-    <mergeCell ref="V81:W81"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="N22:R22"/>
-    <mergeCell ref="N23:R23"/>
-    <mergeCell ref="N24:R24"/>
-    <mergeCell ref="N25:R25"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="N91:R91"/>
-    <mergeCell ref="S91:Y91"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="N86:R86"/>
-    <mergeCell ref="S86:Y86"/>
-    <mergeCell ref="N87:R87"/>
-    <mergeCell ref="S87:Y87"/>
-    <mergeCell ref="N88:R88"/>
-    <mergeCell ref="S88:Y88"/>
-    <mergeCell ref="N89:R89"/>
-    <mergeCell ref="S89:Y89"/>
-    <mergeCell ref="N90:R90"/>
-    <mergeCell ref="S90:Y90"/>
-    <mergeCell ref="H82:L82"/>
-    <mergeCell ref="M82:N82"/>
-    <mergeCell ref="T82:U82"/>
-    <mergeCell ref="V82:W82"/>
-    <mergeCell ref="H83:L83"/>
-    <mergeCell ref="M83:N83"/>
-    <mergeCell ref="O83:P83"/>
-    <mergeCell ref="H84:L84"/>
-    <mergeCell ref="S85:T85"/>
-    <mergeCell ref="N78:R78"/>
-    <mergeCell ref="S78:Y78"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="H54:L54"/>
+    <mergeCell ref="S36:Y36"/>
+    <mergeCell ref="S37:Y37"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="S45:Y45"/>
+    <mergeCell ref="S46:Y46"/>
+    <mergeCell ref="S47:Y47"/>
+    <mergeCell ref="S24:Y24"/>
+    <mergeCell ref="S25:Y25"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="S33:Y33"/>
+    <mergeCell ref="S34:Y34"/>
+    <mergeCell ref="S35:Y35"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="M56:N56"/>
+    <mergeCell ref="H58:L58"/>
+    <mergeCell ref="S59:T59"/>
+    <mergeCell ref="N60:R60"/>
+    <mergeCell ref="S60:Y60"/>
+    <mergeCell ref="S48:Y48"/>
+    <mergeCell ref="S49:Y49"/>
+    <mergeCell ref="S50:Y50"/>
+    <mergeCell ref="N50:R50"/>
+    <mergeCell ref="H57:L57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="T55:U55"/>
+    <mergeCell ref="T56:U56"/>
+    <mergeCell ref="V55:W55"/>
+    <mergeCell ref="V56:W56"/>
+    <mergeCell ref="V57:W57"/>
+    <mergeCell ref="T57:U57"/>
+    <mergeCell ref="N61:R61"/>
+    <mergeCell ref="S61:Y61"/>
+    <mergeCell ref="N62:R62"/>
+    <mergeCell ref="S62:Y62"/>
+    <mergeCell ref="N63:R63"/>
+    <mergeCell ref="S63:Y63"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="S72:T72"/>
+    <mergeCell ref="N73:R73"/>
+    <mergeCell ref="S73:Y73"/>
+    <mergeCell ref="H67:L67"/>
+    <mergeCell ref="H68:L68"/>
+    <mergeCell ref="H69:L69"/>
+    <mergeCell ref="M69:N69"/>
+    <mergeCell ref="H70:L70"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="T69:U69"/>
+    <mergeCell ref="V69:W69"/>
+    <mergeCell ref="T68:U68"/>
+    <mergeCell ref="V68:W68"/>
+    <mergeCell ref="N75:R75"/>
+    <mergeCell ref="S75:Y75"/>
+    <mergeCell ref="N76:R76"/>
+    <mergeCell ref="S76:Y76"/>
+    <mergeCell ref="N77:R77"/>
+    <mergeCell ref="S77:Y77"/>
+    <mergeCell ref="O70:P70"/>
+    <mergeCell ref="N64:R64"/>
+    <mergeCell ref="S64:Y64"/>
+    <mergeCell ref="N65:R65"/>
+    <mergeCell ref="S65:Y65"/>
+    <mergeCell ref="N74:R74"/>
+    <mergeCell ref="S74:Y74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
-Added video folder -Added unfinished trailer - no gameplay in it yet -Altered excel spacing on the Game Data
</commit_message>
<xml_diff>
--- a/documents/Game data.xlsx
+++ b/documents/Game data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dm1\aventale-interactive-gam130\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naomi\Desktop\UNI\GAM130 - Aventale Interactive\aventale-interactive-gam130\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DB4328-C850-404D-948D-6ACD007FEB3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA0FB0-92A0-43B1-B665-6B179161DF63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B55EC6BF-FA38-47AF-9968-4D4850AC5ACB}"/>
   </bookViews>
@@ -770,43 +770,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1133,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C40039-D8C4-497C-BD03-8534292B2959}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1146,8 @@
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="17" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1506,25 +1507,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="70" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="71" t="s">
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -1545,13 +1546,13 @@
       <c r="F3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
     </row>
@@ -1563,13 +1564,13 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
       <c r="M4" t="s">
         <v>37</v>
       </c>
@@ -1599,17 +1600,17 @@
       <c r="F5" s="15">
         <v>10</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="61" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="61"/>
+      <c r="N5" s="66"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -1630,17 +1631,17 @@
       <c r="F6" s="16">
         <v>15</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="61" t="s">
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="61"/>
+      <c r="N6" s="66"/>
       <c r="O6" s="35" t="s">
         <v>41</v>
       </c>
@@ -1669,13 +1670,13 @@
       <c r="F7" s="17">
         <v>25</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
       <c r="M7" t="s">
         <v>49</v>
       </c>
@@ -1710,10 +1711,10 @@
       <c r="N8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S8" s="63" t="s">
+      <c r="S8" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="T8" s="63"/>
+      <c r="T8" s="68"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1728,22 +1729,22 @@
       <c r="J9" s="37"/>
       <c r="K9" s="32"/>
       <c r="L9" s="37"/>
-      <c r="N9" s="60" t="s">
+      <c r="N9" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60" t="s">
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="T9" s="60"/>
-      <c r="U9" s="60"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1769,22 +1770,22 @@
       <c r="J10" s="32"/>
       <c r="K10" s="37"/>
       <c r="L10" s="32"/>
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60" t="s">
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="T10" s="60"/>
-      <c r="U10" s="60"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="60"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1810,20 +1811,20 @@
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="37"/>
-      <c r="N11" s="60" t="s">
+      <c r="N11" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="60"/>
-      <c r="V11" s="60"/>
-      <c r="W11" s="60"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="60"/>
+      <c r="O11" s="62"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="62"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="62"/>
+      <c r="V11" s="62"/>
+      <c r="W11" s="62"/>
+      <c r="X11" s="62"/>
+      <c r="Y11" s="62"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
@@ -1849,20 +1850,20 @@
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="32"/>
-      <c r="N12" s="60" t="s">
+      <c r="N12" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="60"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="60"/>
-      <c r="U12" s="60"/>
-      <c r="V12" s="60"/>
-      <c r="W12" s="60"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="60"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="62"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="62"/>
+      <c r="W12" s="62"/>
+      <c r="X12" s="62"/>
+      <c r="Y12" s="62"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -1888,18 +1889,18 @@
       <c r="J13" s="37"/>
       <c r="K13" s="32"/>
       <c r="L13" s="37"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="60"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="60"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="62"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="62"/>
     </row>
     <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
@@ -1920,13 +1921,13 @@
       <c r="F15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="63" t="s">
+      <c r="H15" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
       <c r="M15" s="33"/>
       <c r="N15" s="33"/>
     </row>
@@ -1938,13 +1939,13 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="H16" s="65" t="s">
+      <c r="H16" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
       <c r="M16" s="40" t="s">
         <v>51</v>
       </c>
@@ -1974,17 +1975,17 @@
       <c r="F17" s="15">
         <v>10</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="61" t="s">
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="61"/>
+      <c r="N17" s="66"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -2005,17 +2006,17 @@
       <c r="F18" s="16">
         <v>15</v>
       </c>
-      <c r="H18" s="65" t="s">
+      <c r="H18" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="61" t="s">
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="61"/>
+      <c r="N18" s="66"/>
       <c r="O18" s="39" t="s">
         <v>53</v>
       </c>
@@ -2044,13 +2045,13 @@
       <c r="F19" s="42">
         <v>25</v>
       </c>
-      <c r="H19" s="65" t="s">
+      <c r="H19" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
       <c r="M19" s="40" t="s">
         <v>52</v>
       </c>
@@ -2085,10 +2086,10 @@
       <c r="N20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S20" s="63" t="s">
+      <c r="S20" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="T20" s="63"/>
+      <c r="T20" s="68"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2103,22 +2104,22 @@
       <c r="J21" s="37"/>
       <c r="K21" s="32"/>
       <c r="L21" s="37"/>
-      <c r="N21" s="60" t="s">
+      <c r="N21" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="60" t="s">
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="T21" s="60"/>
-      <c r="U21" s="60"/>
-      <c r="V21" s="60"/>
-      <c r="W21" s="60"/>
-      <c r="X21" s="60"/>
-      <c r="Y21" s="60"/>
+      <c r="T21" s="62"/>
+      <c r="U21" s="62"/>
+      <c r="V21" s="62"/>
+      <c r="W21" s="62"/>
+      <c r="X21" s="62"/>
+      <c r="Y21" s="62"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
@@ -2144,22 +2145,22 @@
       <c r="J22" s="31"/>
       <c r="K22" s="37"/>
       <c r="L22" s="32"/>
-      <c r="N22" s="60" t="s">
+      <c r="N22" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="60" t="s">
+      <c r="O22" s="62"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="62"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="T22" s="60"/>
-      <c r="U22" s="60"/>
-      <c r="V22" s="60"/>
-      <c r="W22" s="60"/>
-      <c r="X22" s="60"/>
-      <c r="Y22" s="60"/>
+      <c r="T22" s="62"/>
+      <c r="U22" s="62"/>
+      <c r="V22" s="62"/>
+      <c r="W22" s="62"/>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="62"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -2185,22 +2186,22 @@
       <c r="J23" s="31"/>
       <c r="K23" s="38"/>
       <c r="L23" s="37"/>
-      <c r="N23" s="60" t="s">
+      <c r="N23" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60" t="s">
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="T23" s="60"/>
-      <c r="U23" s="60"/>
-      <c r="V23" s="60"/>
-      <c r="W23" s="60"/>
-      <c r="X23" s="60"/>
-      <c r="Y23" s="60"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62"/>
+      <c r="W23" s="62"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="62"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
@@ -2226,20 +2227,20 @@
       <c r="J24" s="38"/>
       <c r="K24" s="37"/>
       <c r="L24" s="32"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60" t="s">
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="62"/>
+      <c r="R24" s="62"/>
+      <c r="S24" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="60"/>
-      <c r="W24" s="60"/>
-      <c r="X24" s="60"/>
-      <c r="Y24" s="60"/>
+      <c r="T24" s="62"/>
+      <c r="U24" s="62"/>
+      <c r="V24" s="62"/>
+      <c r="W24" s="62"/>
+      <c r="X24" s="62"/>
+      <c r="Y24" s="62"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -2265,20 +2266,20 @@
       <c r="J25" s="37"/>
       <c r="K25" s="32"/>
       <c r="L25" s="37"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60" t="s">
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
+      <c r="S25" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="60"/>
-      <c r="W25" s="60"/>
-      <c r="X25" s="60"/>
-      <c r="Y25" s="60"/>
+      <c r="T25" s="62"/>
+      <c r="U25" s="62"/>
+      <c r="V25" s="62"/>
+      <c r="W25" s="62"/>
+      <c r="X25" s="62"/>
+      <c r="Y25" s="62"/>
     </row>
     <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
@@ -2299,13 +2300,13 @@
       <c r="F27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="63" t="s">
+      <c r="H27" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="63"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
       <c r="M27" s="33"/>
       <c r="N27" s="33"/>
     </row>
@@ -2317,13 +2318,13 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="H28" s="68" t="s">
+      <c r="H28" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
       <c r="M28" s="43" t="s">
         <v>51</v>
       </c>
@@ -2354,17 +2355,17 @@
       <c r="F29" s="15">
         <v>10</v>
       </c>
-      <c r="H29" s="68" t="s">
+      <c r="H29" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="69" t="s">
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="N29" s="69"/>
+      <c r="N29" s="72"/>
       <c r="O29" s="43"/>
       <c r="P29" s="43"/>
     </row>
@@ -2387,17 +2388,17 @@
       <c r="F30" s="16">
         <v>15</v>
       </c>
-      <c r="H30" s="68" t="s">
+      <c r="H30" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="69" t="s">
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="N30" s="69"/>
+      <c r="N30" s="72"/>
       <c r="O30" s="44" t="s">
         <v>53</v>
       </c>
@@ -2426,13 +2427,13 @@
       <c r="F31" s="41">
         <v>20</v>
       </c>
-      <c r="H31" s="65" t="s">
+      <c r="H31" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
       <c r="M31" s="40" t="s">
         <v>64</v>
       </c>
@@ -2470,10 +2471,10 @@
       <c r="N32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S32" s="63" t="s">
+      <c r="S32" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="T32" s="63"/>
+      <c r="T32" s="68"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2488,22 +2489,22 @@
       <c r="J33" s="37"/>
       <c r="K33" s="32"/>
       <c r="L33" s="37"/>
-      <c r="N33" s="60" t="s">
+      <c r="N33" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="O33" s="60"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="60" t="s">
+      <c r="O33" s="62"/>
+      <c r="P33" s="62"/>
+      <c r="Q33" s="62"/>
+      <c r="R33" s="62"/>
+      <c r="S33" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="T33" s="60"/>
-      <c r="U33" s="60"/>
-      <c r="V33" s="60"/>
-      <c r="W33" s="60"/>
-      <c r="X33" s="60"/>
-      <c r="Y33" s="60"/>
+      <c r="T33" s="62"/>
+      <c r="U33" s="62"/>
+      <c r="V33" s="62"/>
+      <c r="W33" s="62"/>
+      <c r="X33" s="62"/>
+      <c r="Y33" s="62"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
@@ -2529,22 +2530,22 @@
       <c r="J34" s="31"/>
       <c r="K34" s="37"/>
       <c r="L34" s="32"/>
-      <c r="N34" s="60" t="s">
+      <c r="N34" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="O34" s="60"/>
-      <c r="P34" s="60"/>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="60"/>
-      <c r="S34" s="60" t="s">
+      <c r="O34" s="62"/>
+      <c r="P34" s="62"/>
+      <c r="Q34" s="62"/>
+      <c r="R34" s="62"/>
+      <c r="S34" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="T34" s="60"/>
-      <c r="U34" s="60"/>
-      <c r="V34" s="60"/>
-      <c r="W34" s="60"/>
-      <c r="X34" s="60"/>
-      <c r="Y34" s="60"/>
+      <c r="T34" s="62"/>
+      <c r="U34" s="62"/>
+      <c r="V34" s="62"/>
+      <c r="W34" s="62"/>
+      <c r="X34" s="62"/>
+      <c r="Y34" s="62"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
@@ -2570,20 +2571,20 @@
       <c r="J35" s="31"/>
       <c r="K35" s="38"/>
       <c r="L35" s="37"/>
-      <c r="N35" s="60"/>
-      <c r="O35" s="60"/>
-      <c r="P35" s="60"/>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="60" t="s">
+      <c r="N35" s="62"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
+      <c r="Q35" s="62"/>
+      <c r="R35" s="62"/>
+      <c r="S35" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="T35" s="60"/>
-      <c r="U35" s="60"/>
-      <c r="V35" s="60"/>
-      <c r="W35" s="60"/>
-      <c r="X35" s="60"/>
-      <c r="Y35" s="60"/>
+      <c r="T35" s="62"/>
+      <c r="U35" s="62"/>
+      <c r="V35" s="62"/>
+      <c r="W35" s="62"/>
+      <c r="X35" s="62"/>
+      <c r="Y35" s="62"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
@@ -2609,18 +2610,18 @@
       <c r="J36" s="38"/>
       <c r="K36" s="37"/>
       <c r="L36" s="32"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="60"/>
-      <c r="P36" s="60"/>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="60"/>
-      <c r="S36" s="60"/>
-      <c r="T36" s="60"/>
-      <c r="U36" s="60"/>
-      <c r="V36" s="60"/>
-      <c r="W36" s="60"/>
-      <c r="X36" s="60"/>
-      <c r="Y36" s="60"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="62"/>
+      <c r="T36" s="62"/>
+      <c r="U36" s="62"/>
+      <c r="V36" s="62"/>
+      <c r="W36" s="62"/>
+      <c r="X36" s="62"/>
+      <c r="Y36" s="62"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
@@ -2646,18 +2647,18 @@
       <c r="J37" s="37"/>
       <c r="K37" s="32"/>
       <c r="L37" s="37"/>
-      <c r="N37" s="60"/>
-      <c r="O37" s="60"/>
-      <c r="P37" s="60"/>
-      <c r="Q37" s="60"/>
-      <c r="R37" s="60"/>
-      <c r="S37" s="60"/>
-      <c r="T37" s="60"/>
-      <c r="U37" s="60"/>
-      <c r="V37" s="60"/>
-      <c r="W37" s="60"/>
-      <c r="X37" s="60"/>
-      <c r="Y37" s="60"/>
+      <c r="N37" s="62"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
+      <c r="Q37" s="62"/>
+      <c r="R37" s="62"/>
+      <c r="S37" s="62"/>
+      <c r="T37" s="62"/>
+      <c r="U37" s="62"/>
+      <c r="V37" s="62"/>
+      <c r="W37" s="62"/>
+      <c r="X37" s="62"/>
+      <c r="Y37" s="62"/>
     </row>
     <row r="39" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
@@ -2675,13 +2676,13 @@
       <c r="E39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="63" t="s">
+      <c r="H39" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="63"/>
-      <c r="J39" s="63"/>
-      <c r="K39" s="63"/>
-      <c r="L39" s="63"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
       <c r="M39" s="33"/>
       <c r="N39" s="33"/>
     </row>
@@ -2693,13 +2694,13 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="H40" s="64" t="s">
+      <c r="H40" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="I40" s="64"/>
-      <c r="J40" s="64"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="65"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="65"/>
       <c r="M40" t="s">
         <v>70</v>
       </c>
@@ -2729,17 +2730,17 @@
       <c r="E41" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="64" t="s">
+      <c r="H41" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="I41" s="64"/>
-      <c r="J41" s="64"/>
-      <c r="K41" s="64"/>
-      <c r="L41" s="64"/>
-      <c r="M41" s="61" t="s">
+      <c r="I41" s="65"/>
+      <c r="J41" s="65"/>
+      <c r="K41" s="65"/>
+      <c r="L41" s="65"/>
+      <c r="M41" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="N41" s="61"/>
+      <c r="N41" s="66"/>
       <c r="O41" t="s">
         <v>72</v>
       </c>
@@ -2779,13 +2780,13 @@
       <c r="E43" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H43" s="68" t="s">
+      <c r="H43" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
       <c r="M43" s="43" t="s">
         <v>64</v>
       </c>
@@ -2818,10 +2819,10 @@
       <c r="N44" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S44" s="63" t="s">
+      <c r="S44" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="T44" s="63"/>
+      <c r="T44" s="68"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -2836,22 +2837,22 @@
       <c r="J45" s="37"/>
       <c r="K45" s="32"/>
       <c r="L45" s="37"/>
-      <c r="N45" s="60" t="s">
+      <c r="N45" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="O45" s="60"/>
-      <c r="P45" s="60"/>
-      <c r="Q45" s="60"/>
-      <c r="R45" s="60"/>
-      <c r="S45" s="60" t="s">
+      <c r="O45" s="62"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="62"/>
+      <c r="R45" s="62"/>
+      <c r="S45" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="T45" s="60"/>
-      <c r="U45" s="60"/>
-      <c r="V45" s="60"/>
-      <c r="W45" s="60"/>
-      <c r="X45" s="60"/>
-      <c r="Y45" s="60"/>
+      <c r="T45" s="62"/>
+      <c r="U45" s="62"/>
+      <c r="V45" s="62"/>
+      <c r="W45" s="62"/>
+      <c r="X45" s="62"/>
+      <c r="Y45" s="62"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
@@ -2874,22 +2875,22 @@
       <c r="J46" s="31"/>
       <c r="K46" s="37"/>
       <c r="L46" s="32"/>
-      <c r="N46" s="60" t="s">
+      <c r="N46" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="O46" s="60"/>
-      <c r="P46" s="60"/>
-      <c r="Q46" s="60"/>
-      <c r="R46" s="60"/>
-      <c r="S46" s="60" t="s">
+      <c r="O46" s="62"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="62"/>
+      <c r="R46" s="62"/>
+      <c r="S46" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="T46" s="60"/>
-      <c r="U46" s="60"/>
-      <c r="V46" s="60"/>
-      <c r="W46" s="60"/>
-      <c r="X46" s="60"/>
-      <c r="Y46" s="60"/>
+      <c r="T46" s="62"/>
+      <c r="U46" s="62"/>
+      <c r="V46" s="62"/>
+      <c r="W46" s="62"/>
+      <c r="X46" s="62"/>
+      <c r="Y46" s="62"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H47" s="37"/>
@@ -2897,22 +2898,22 @@
       <c r="J47" s="31"/>
       <c r="K47" s="38"/>
       <c r="L47" s="37"/>
-      <c r="N47" s="60" t="s">
+      <c r="N47" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="O47" s="60"/>
-      <c r="P47" s="60"/>
-      <c r="Q47" s="60"/>
-      <c r="R47" s="60"/>
-      <c r="S47" s="60" t="s">
+      <c r="O47" s="62"/>
+      <c r="P47" s="62"/>
+      <c r="Q47" s="62"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="T47" s="60"/>
-      <c r="U47" s="60"/>
-      <c r="V47" s="60"/>
-      <c r="W47" s="60"/>
-      <c r="X47" s="60"/>
-      <c r="Y47" s="60"/>
+      <c r="T47" s="62"/>
+      <c r="U47" s="62"/>
+      <c r="V47" s="62"/>
+      <c r="W47" s="62"/>
+      <c r="X47" s="62"/>
+      <c r="Y47" s="62"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H48" s="32"/>
@@ -2920,20 +2921,20 @@
       <c r="J48" s="38"/>
       <c r="K48" s="37"/>
       <c r="L48" s="32"/>
-      <c r="N48" s="60"/>
-      <c r="O48" s="60"/>
-      <c r="P48" s="60"/>
-      <c r="Q48" s="60"/>
-      <c r="R48" s="60"/>
-      <c r="S48" s="60" t="s">
+      <c r="N48" s="62"/>
+      <c r="O48" s="62"/>
+      <c r="P48" s="62"/>
+      <c r="Q48" s="62"/>
+      <c r="R48" s="62"/>
+      <c r="S48" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="T48" s="60"/>
-      <c r="U48" s="60"/>
-      <c r="V48" s="60"/>
-      <c r="W48" s="60"/>
-      <c r="X48" s="60"/>
-      <c r="Y48" s="60"/>
+      <c r="T48" s="62"/>
+      <c r="U48" s="62"/>
+      <c r="V48" s="62"/>
+      <c r="W48" s="62"/>
+      <c r="X48" s="62"/>
+      <c r="Y48" s="62"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H49" s="37"/>
@@ -2941,42 +2942,42 @@
       <c r="J49" s="37"/>
       <c r="K49" s="32"/>
       <c r="L49" s="37"/>
-      <c r="N49" s="60"/>
-      <c r="O49" s="60"/>
-      <c r="P49" s="60"/>
-      <c r="Q49" s="60"/>
-      <c r="R49" s="60"/>
-      <c r="S49" s="60" t="s">
+      <c r="N49" s="62"/>
+      <c r="O49" s="62"/>
+      <c r="P49" s="62"/>
+      <c r="Q49" s="62"/>
+      <c r="R49" s="62"/>
+      <c r="S49" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="T49" s="60"/>
-      <c r="U49" s="60"/>
-      <c r="V49" s="60"/>
-      <c r="W49" s="60"/>
-      <c r="X49" s="60"/>
-      <c r="Y49" s="60"/>
+      <c r="T49" s="62"/>
+      <c r="U49" s="62"/>
+      <c r="V49" s="62"/>
+      <c r="W49" s="62"/>
+      <c r="X49" s="62"/>
+      <c r="Y49" s="62"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N50" s="62"/>
-      <c r="O50" s="62"/>
-      <c r="P50" s="62"/>
-      <c r="Q50" s="62"/>
-      <c r="R50" s="62"/>
-      <c r="S50" s="62" t="s">
+      <c r="N50" s="60"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="60"/>
+      <c r="Q50" s="60"/>
+      <c r="R50" s="60"/>
+      <c r="S50" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="T50" s="62"/>
-      <c r="U50" s="62"/>
-      <c r="V50" s="62"/>
-      <c r="W50" s="62"/>
-      <c r="X50" s="62"/>
-      <c r="Y50" s="62"/>
+      <c r="T50" s="60"/>
+      <c r="U50" s="60"/>
+      <c r="V50" s="60"/>
+      <c r="W50" s="60"/>
+      <c r="X50" s="60"/>
+      <c r="Y50" s="60"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A52" s="67" t="s">
+      <c r="A52" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="67"/>
+      <c r="B52" s="61"/>
     </row>
     <row r="54" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
@@ -2994,13 +2995,13 @@
       <c r="E54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="63" t="s">
+      <c r="H54" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="I54" s="63"/>
-      <c r="J54" s="63"/>
-      <c r="K54" s="63"/>
-      <c r="L54" s="63"/>
+      <c r="I54" s="68"/>
+      <c r="J54" s="68"/>
+      <c r="K54" s="68"/>
+      <c r="L54" s="68"/>
       <c r="M54" s="33"/>
       <c r="N54" s="33"/>
     </row>
@@ -3012,13 +3013,13 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="H55" s="64" t="s">
+      <c r="H55" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="I55" s="64"/>
-      <c r="J55" s="64"/>
-      <c r="K55" s="64"/>
-      <c r="L55" s="64"/>
+      <c r="I55" s="65"/>
+      <c r="J55" s="65"/>
+      <c r="K55" s="65"/>
+      <c r="L55" s="65"/>
       <c r="M55" t="s">
         <v>70</v>
       </c>
@@ -3031,14 +3032,14 @@
       <c r="P55" t="s">
         <v>67</v>
       </c>
-      <c r="T55" s="63" t="s">
+      <c r="T55" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="U55" s="63"/>
-      <c r="V55" s="63" t="s">
+      <c r="U55" s="68"/>
+      <c r="V55" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="W55" s="63"/>
+      <c r="W55" s="68"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
@@ -3056,31 +3057,31 @@
       <c r="E56" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="64" t="s">
+      <c r="H56" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="I56" s="64"/>
-      <c r="J56" s="64"/>
-      <c r="K56" s="64"/>
-      <c r="L56" s="64"/>
-      <c r="M56" s="61" t="s">
+      <c r="I56" s="65"/>
+      <c r="J56" s="65"/>
+      <c r="K56" s="65"/>
+      <c r="L56" s="65"/>
+      <c r="M56" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="N56" s="61"/>
+      <c r="N56" s="66"/>
       <c r="O56" t="s">
         <v>72</v>
       </c>
       <c r="S56" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="T56" s="67" t="s">
+      <c r="T56" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="U56" s="67"/>
-      <c r="V56" s="67" t="s">
+      <c r="U56" s="61"/>
+      <c r="V56" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="W56" s="67"/>
+      <c r="W56" s="61"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
@@ -3098,34 +3099,34 @@
       <c r="E57" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H57" s="64" t="s">
+      <c r="H57" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="I57" s="64"/>
-      <c r="J57" s="64"/>
-      <c r="K57" s="64"/>
-      <c r="L57" s="64"/>
-      <c r="M57" s="61" t="s">
+      <c r="I57" s="65"/>
+      <c r="J57" s="65"/>
+      <c r="K57" s="65"/>
+      <c r="L57" s="65"/>
+      <c r="M57" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="N57" s="61"/>
-      <c r="O57" s="61" t="s">
+      <c r="N57" s="66"/>
+      <c r="O57" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="P57" s="61"/>
+      <c r="P57" s="66"/>
       <c r="Q57" s="33"/>
       <c r="R57" s="33"/>
       <c r="S57" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="T57" s="67" t="s">
+      <c r="T57" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="U57" s="67"/>
-      <c r="V57" s="67" t="s">
+      <c r="U57" s="61"/>
+      <c r="V57" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="W57" s="67"/>
+      <c r="W57" s="61"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
@@ -3143,13 +3144,13 @@
       <c r="E58" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H58" s="68" t="s">
+      <c r="H58" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="I58" s="68"/>
-      <c r="J58" s="68"/>
-      <c r="K58" s="68"/>
-      <c r="L58" s="68"/>
+      <c r="I58" s="67"/>
+      <c r="J58" s="67"/>
+      <c r="K58" s="67"/>
+      <c r="L58" s="67"/>
       <c r="M58" s="43" t="s">
         <v>64</v>
       </c>
@@ -3182,10 +3183,10 @@
       <c r="N59" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S59" s="63" t="s">
+      <c r="S59" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="T59" s="63"/>
+      <c r="T59" s="68"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -3200,22 +3201,22 @@
       <c r="J60" s="37"/>
       <c r="K60" s="32"/>
       <c r="L60" s="37"/>
-      <c r="N60" s="60" t="s">
+      <c r="N60" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="O60" s="60"/>
-      <c r="P60" s="60"/>
-      <c r="Q60" s="60"/>
-      <c r="R60" s="60"/>
-      <c r="S60" s="60" t="s">
+      <c r="O60" s="62"/>
+      <c r="P60" s="62"/>
+      <c r="Q60" s="62"/>
+      <c r="R60" s="62"/>
+      <c r="S60" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="T60" s="60"/>
-      <c r="U60" s="60"/>
-      <c r="V60" s="60"/>
-      <c r="W60" s="60"/>
-      <c r="X60" s="60"/>
-      <c r="Y60" s="60"/>
+      <c r="T60" s="62"/>
+      <c r="U60" s="62"/>
+      <c r="V60" s="62"/>
+      <c r="W60" s="62"/>
+      <c r="X60" s="62"/>
+      <c r="Y60" s="62"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
@@ -3238,22 +3239,22 @@
       <c r="J61" s="31"/>
       <c r="K61" s="37"/>
       <c r="L61" s="32"/>
-      <c r="N61" s="60" t="s">
+      <c r="N61" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="O61" s="60"/>
-      <c r="P61" s="60"/>
-      <c r="Q61" s="60"/>
-      <c r="R61" s="60"/>
-      <c r="S61" s="60" t="s">
+      <c r="O61" s="62"/>
+      <c r="P61" s="62"/>
+      <c r="Q61" s="62"/>
+      <c r="R61" s="62"/>
+      <c r="S61" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="T61" s="60"/>
-      <c r="U61" s="60"/>
-      <c r="V61" s="60"/>
-      <c r="W61" s="60"/>
-      <c r="X61" s="60"/>
-      <c r="Y61" s="60"/>
+      <c r="T61" s="62"/>
+      <c r="U61" s="62"/>
+      <c r="V61" s="62"/>
+      <c r="W61" s="62"/>
+      <c r="X61" s="62"/>
+      <c r="Y61" s="62"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
@@ -3276,22 +3277,22 @@
       <c r="J62" s="31"/>
       <c r="K62" s="38"/>
       <c r="L62" s="37"/>
-      <c r="N62" s="60" t="s">
+      <c r="N62" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="O62" s="60"/>
-      <c r="P62" s="60"/>
-      <c r="Q62" s="60"/>
-      <c r="R62" s="60"/>
-      <c r="S62" s="60" t="s">
+      <c r="O62" s="62"/>
+      <c r="P62" s="62"/>
+      <c r="Q62" s="62"/>
+      <c r="R62" s="62"/>
+      <c r="S62" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="T62" s="60"/>
-      <c r="U62" s="60"/>
-      <c r="V62" s="60"/>
-      <c r="W62" s="60"/>
-      <c r="X62" s="60"/>
-      <c r="Y62" s="60"/>
+      <c r="T62" s="62"/>
+      <c r="U62" s="62"/>
+      <c r="V62" s="62"/>
+      <c r="W62" s="62"/>
+      <c r="X62" s="62"/>
+      <c r="Y62" s="62"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H63" s="32"/>
@@ -3299,22 +3300,22 @@
       <c r="J63" s="38"/>
       <c r="K63" s="37"/>
       <c r="L63" s="32"/>
-      <c r="N63" s="60" t="s">
+      <c r="N63" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="O63" s="60"/>
-      <c r="P63" s="60"/>
-      <c r="Q63" s="60"/>
-      <c r="R63" s="60"/>
-      <c r="S63" s="60" t="s">
+      <c r="O63" s="62"/>
+      <c r="P63" s="62"/>
+      <c r="Q63" s="62"/>
+      <c r="R63" s="62"/>
+      <c r="S63" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="T63" s="60"/>
-      <c r="U63" s="60"/>
-      <c r="V63" s="60"/>
-      <c r="W63" s="60"/>
-      <c r="X63" s="60"/>
-      <c r="Y63" s="60"/>
+      <c r="T63" s="62"/>
+      <c r="U63" s="62"/>
+      <c r="V63" s="62"/>
+      <c r="W63" s="62"/>
+      <c r="X63" s="62"/>
+      <c r="Y63" s="62"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H64" s="37"/>
@@ -3322,38 +3323,38 @@
       <c r="J64" s="37"/>
       <c r="K64" s="32"/>
       <c r="L64" s="37"/>
-      <c r="N64" s="60" t="s">
+      <c r="N64" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="O64" s="60"/>
-      <c r="P64" s="60"/>
-      <c r="Q64" s="60"/>
-      <c r="R64" s="60"/>
-      <c r="S64" s="60" t="s">
+      <c r="O64" s="62"/>
+      <c r="P64" s="62"/>
+      <c r="Q64" s="62"/>
+      <c r="R64" s="62"/>
+      <c r="S64" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="T64" s="60"/>
-      <c r="U64" s="60"/>
-      <c r="V64" s="60"/>
-      <c r="W64" s="60"/>
-      <c r="X64" s="60"/>
-      <c r="Y64" s="60"/>
+      <c r="T64" s="62"/>
+      <c r="U64" s="62"/>
+      <c r="V64" s="62"/>
+      <c r="W64" s="62"/>
+      <c r="X64" s="62"/>
+      <c r="Y64" s="62"/>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N65" s="62"/>
-      <c r="O65" s="62"/>
-      <c r="P65" s="62"/>
-      <c r="Q65" s="62"/>
-      <c r="R65" s="62"/>
-      <c r="S65" s="62" t="s">
+      <c r="N65" s="60"/>
+      <c r="O65" s="60"/>
+      <c r="P65" s="60"/>
+      <c r="Q65" s="60"/>
+      <c r="R65" s="60"/>
+      <c r="S65" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="T65" s="62"/>
-      <c r="U65" s="62"/>
-      <c r="V65" s="62"/>
-      <c r="W65" s="62"/>
-      <c r="X65" s="62"/>
-      <c r="Y65" s="62"/>
+      <c r="T65" s="60"/>
+      <c r="U65" s="60"/>
+      <c r="V65" s="60"/>
+      <c r="W65" s="60"/>
+      <c r="X65" s="60"/>
+      <c r="Y65" s="60"/>
     </row>
     <row r="67" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="26" t="s">
@@ -3371,13 +3372,13 @@
       <c r="E67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="63" t="s">
+      <c r="H67" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="I67" s="63"/>
-      <c r="J67" s="63"/>
-      <c r="K67" s="63"/>
-      <c r="L67" s="63"/>
+      <c r="I67" s="68"/>
+      <c r="J67" s="68"/>
+      <c r="K67" s="68"/>
+      <c r="L67" s="68"/>
       <c r="M67" s="33"/>
       <c r="N67" s="33"/>
     </row>
@@ -3389,13 +3390,13 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="H68" s="64" t="s">
+      <c r="H68" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="I68" s="64"/>
-      <c r="J68" s="64"/>
-      <c r="K68" s="64"/>
-      <c r="L68" s="64"/>
+      <c r="I68" s="65"/>
+      <c r="J68" s="65"/>
+      <c r="K68" s="65"/>
+      <c r="L68" s="65"/>
       <c r="M68" t="s">
         <v>70</v>
       </c>
@@ -3408,14 +3409,14 @@
       <c r="P68" t="s">
         <v>67</v>
       </c>
-      <c r="T68" s="63" t="s">
+      <c r="T68" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="U68" s="63"/>
-      <c r="V68" s="63" t="s">
+      <c r="U68" s="68"/>
+      <c r="V68" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="W68" s="63"/>
+      <c r="W68" s="68"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
@@ -3433,31 +3434,31 @@
       <c r="E69" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H69" s="65" t="s">
+      <c r="H69" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="I69" s="65"/>
-      <c r="J69" s="65"/>
-      <c r="K69" s="65"/>
-      <c r="L69" s="65"/>
-      <c r="M69" s="66" t="s">
+      <c r="I69" s="63"/>
+      <c r="J69" s="63"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="63"/>
+      <c r="M69" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="N69" s="66"/>
+      <c r="N69" s="64"/>
       <c r="O69" t="s">
         <v>72</v>
       </c>
       <c r="S69" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="T69" s="67" t="s">
+      <c r="T69" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="U69" s="67"/>
-      <c r="V69" s="67" t="s">
+      <c r="U69" s="61"/>
+      <c r="V69" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="W69" s="67"/>
+      <c r="W69" s="61"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
@@ -3475,21 +3476,21 @@
       <c r="E70" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H70" s="64" t="s">
+      <c r="H70" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="I70" s="64"/>
-      <c r="J70" s="64"/>
-      <c r="K70" s="64"/>
-      <c r="L70" s="64"/>
-      <c r="M70" s="61" t="s">
+      <c r="I70" s="65"/>
+      <c r="J70" s="65"/>
+      <c r="K70" s="65"/>
+      <c r="L70" s="65"/>
+      <c r="M70" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="N70" s="61"/>
-      <c r="O70" s="61" t="s">
+      <c r="N70" s="66"/>
+      <c r="O70" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="P70" s="61"/>
+      <c r="P70" s="66"/>
       <c r="Q70" s="33"/>
       <c r="R70" s="33"/>
     </row>
@@ -3509,13 +3510,13 @@
       <c r="E71" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H71" s="68" t="s">
+      <c r="H71" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="I71" s="68"/>
-      <c r="J71" s="68"/>
-      <c r="K71" s="68"/>
-      <c r="L71" s="68"/>
+      <c r="I71" s="67"/>
+      <c r="J71" s="67"/>
+      <c r="K71" s="67"/>
+      <c r="L71" s="67"/>
       <c r="M71" s="43" t="s">
         <v>64</v>
       </c>
@@ -3548,10 +3549,10 @@
       <c r="N72" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S72" s="63" t="s">
+      <c r="S72" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="T72" s="63"/>
+      <c r="T72" s="68"/>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -3566,22 +3567,22 @@
       <c r="J73" s="37"/>
       <c r="K73" s="32"/>
       <c r="L73" s="37"/>
-      <c r="N73" s="60" t="s">
+      <c r="N73" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="O73" s="60"/>
-      <c r="P73" s="60"/>
-      <c r="Q73" s="60"/>
-      <c r="R73" s="60"/>
-      <c r="S73" s="60" t="s">
+      <c r="O73" s="62"/>
+      <c r="P73" s="62"/>
+      <c r="Q73" s="62"/>
+      <c r="R73" s="62"/>
+      <c r="S73" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="T73" s="60"/>
-      <c r="U73" s="60"/>
-      <c r="V73" s="60"/>
-      <c r="W73" s="60"/>
-      <c r="X73" s="60"/>
-      <c r="Y73" s="60"/>
+      <c r="T73" s="62"/>
+      <c r="U73" s="62"/>
+      <c r="V73" s="62"/>
+      <c r="W73" s="62"/>
+      <c r="X73" s="62"/>
+      <c r="Y73" s="62"/>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
@@ -3604,20 +3605,20 @@
       <c r="J74" s="31"/>
       <c r="K74" s="37"/>
       <c r="L74" s="32"/>
-      <c r="N74" s="60" t="s">
+      <c r="N74" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="O74" s="60"/>
-      <c r="P74" s="60"/>
-      <c r="Q74" s="60"/>
-      <c r="R74" s="60"/>
-      <c r="S74" s="60"/>
-      <c r="T74" s="60"/>
-      <c r="U74" s="60"/>
-      <c r="V74" s="60"/>
-      <c r="W74" s="60"/>
-      <c r="X74" s="60"/>
-      <c r="Y74" s="60"/>
+      <c r="O74" s="62"/>
+      <c r="P74" s="62"/>
+      <c r="Q74" s="62"/>
+      <c r="R74" s="62"/>
+      <c r="S74" s="62"/>
+      <c r="T74" s="62"/>
+      <c r="U74" s="62"/>
+      <c r="V74" s="62"/>
+      <c r="W74" s="62"/>
+      <c r="X74" s="62"/>
+      <c r="Y74" s="62"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
@@ -3640,18 +3641,18 @@
       <c r="J75" s="31"/>
       <c r="K75" s="38"/>
       <c r="L75" s="37"/>
-      <c r="N75" s="60"/>
-      <c r="O75" s="60"/>
-      <c r="P75" s="60"/>
-      <c r="Q75" s="60"/>
-      <c r="R75" s="60"/>
-      <c r="S75" s="60"/>
-      <c r="T75" s="60"/>
-      <c r="U75" s="60"/>
-      <c r="V75" s="60"/>
-      <c r="W75" s="60"/>
-      <c r="X75" s="60"/>
-      <c r="Y75" s="60"/>
+      <c r="N75" s="62"/>
+      <c r="O75" s="62"/>
+      <c r="P75" s="62"/>
+      <c r="Q75" s="62"/>
+      <c r="R75" s="62"/>
+      <c r="S75" s="62"/>
+      <c r="T75" s="62"/>
+      <c r="U75" s="62"/>
+      <c r="V75" s="62"/>
+      <c r="W75" s="62"/>
+      <c r="X75" s="62"/>
+      <c r="Y75" s="62"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H76" s="32"/>
@@ -3659,18 +3660,18 @@
       <c r="J76" s="38"/>
       <c r="K76" s="37"/>
       <c r="L76" s="32"/>
-      <c r="N76" s="60"/>
-      <c r="O76" s="60"/>
-      <c r="P76" s="60"/>
-      <c r="Q76" s="60"/>
-      <c r="R76" s="60"/>
-      <c r="S76" s="60"/>
-      <c r="T76" s="60"/>
-      <c r="U76" s="60"/>
-      <c r="V76" s="60"/>
-      <c r="W76" s="60"/>
-      <c r="X76" s="60"/>
-      <c r="Y76" s="60"/>
+      <c r="N76" s="62"/>
+      <c r="O76" s="62"/>
+      <c r="P76" s="62"/>
+      <c r="Q76" s="62"/>
+      <c r="R76" s="62"/>
+      <c r="S76" s="62"/>
+      <c r="T76" s="62"/>
+      <c r="U76" s="62"/>
+      <c r="V76" s="62"/>
+      <c r="W76" s="62"/>
+      <c r="X76" s="62"/>
+      <c r="Y76" s="62"/>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H77" s="37"/>
@@ -3678,36 +3679,36 @@
       <c r="J77" s="37"/>
       <c r="K77" s="32"/>
       <c r="L77" s="37"/>
-      <c r="N77" s="60"/>
-      <c r="O77" s="60"/>
-      <c r="P77" s="60"/>
-      <c r="Q77" s="60"/>
-      <c r="R77" s="60"/>
-      <c r="S77" s="60"/>
-      <c r="T77" s="60"/>
-      <c r="U77" s="60"/>
-      <c r="V77" s="60"/>
-      <c r="W77" s="60"/>
-      <c r="X77" s="60"/>
-      <c r="Y77" s="60"/>
+      <c r="N77" s="62"/>
+      <c r="O77" s="62"/>
+      <c r="P77" s="62"/>
+      <c r="Q77" s="62"/>
+      <c r="R77" s="62"/>
+      <c r="S77" s="62"/>
+      <c r="T77" s="62"/>
+      <c r="U77" s="62"/>
+      <c r="V77" s="62"/>
+      <c r="W77" s="62"/>
+      <c r="X77" s="62"/>
+      <c r="Y77" s="62"/>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A78" s="67" t="s">
+      <c r="A78" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="B78" s="67"/>
-      <c r="N78" s="62"/>
-      <c r="O78" s="62"/>
-      <c r="P78" s="62"/>
-      <c r="Q78" s="62"/>
-      <c r="R78" s="62"/>
-      <c r="S78" s="62"/>
-      <c r="T78" s="62"/>
-      <c r="U78" s="62"/>
-      <c r="V78" s="62"/>
-      <c r="W78" s="62"/>
-      <c r="X78" s="62"/>
-      <c r="Y78" s="62"/>
+      <c r="B78" s="61"/>
+      <c r="N78" s="60"/>
+      <c r="O78" s="60"/>
+      <c r="P78" s="60"/>
+      <c r="Q78" s="60"/>
+      <c r="R78" s="60"/>
+      <c r="S78" s="60"/>
+      <c r="T78" s="60"/>
+      <c r="U78" s="60"/>
+      <c r="V78" s="60"/>
+      <c r="W78" s="60"/>
+      <c r="X78" s="60"/>
+      <c r="Y78" s="60"/>
     </row>
     <row r="80" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="26" t="s">
@@ -3725,13 +3726,13 @@
       <c r="E80" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H80" s="63" t="s">
+      <c r="H80" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="I80" s="63"/>
-      <c r="J80" s="63"/>
-      <c r="K80" s="63"/>
-      <c r="L80" s="63"/>
+      <c r="I80" s="68"/>
+      <c r="J80" s="68"/>
+      <c r="K80" s="68"/>
+      <c r="L80" s="68"/>
       <c r="M80" s="33"/>
       <c r="N80" s="33"/>
     </row>
@@ -3743,13 +3744,13 @@
       <c r="C81" s="25"/>
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
-      <c r="H81" s="64" t="s">
+      <c r="H81" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="I81" s="64"/>
-      <c r="J81" s="64"/>
-      <c r="K81" s="64"/>
-      <c r="L81" s="64"/>
+      <c r="I81" s="65"/>
+      <c r="J81" s="65"/>
+      <c r="K81" s="65"/>
+      <c r="L81" s="65"/>
       <c r="M81" t="s">
         <v>70</v>
       </c>
@@ -3762,14 +3763,14 @@
       <c r="P81" t="s">
         <v>67</v>
       </c>
-      <c r="T81" s="63" t="s">
+      <c r="T81" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="U81" s="63"/>
-      <c r="V81" s="63" t="s">
+      <c r="U81" s="68"/>
+      <c r="V81" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="W81" s="63"/>
+      <c r="W81" s="68"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
@@ -3787,17 +3788,17 @@
       <c r="E82" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H82" s="65" t="s">
+      <c r="H82" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="I82" s="65"/>
-      <c r="J82" s="65"/>
-      <c r="K82" s="65"/>
-      <c r="L82" s="65"/>
-      <c r="M82" s="66" t="s">
+      <c r="I82" s="63"/>
+      <c r="J82" s="63"/>
+      <c r="K82" s="63"/>
+      <c r="L82" s="63"/>
+      <c r="M82" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="N82" s="66"/>
+      <c r="N82" s="64"/>
       <c r="O82" t="s">
         <v>72</v>
       </c>
@@ -3807,14 +3808,14 @@
       <c r="S82" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="T82" s="67" t="s">
+      <c r="T82" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="U82" s="67"/>
-      <c r="V82" s="67" t="s">
+      <c r="U82" s="61"/>
+      <c r="V82" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="W82" s="67"/>
+      <c r="W82" s="61"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
@@ -3832,21 +3833,21 @@
       <c r="E83" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H83" s="64" t="s">
+      <c r="H83" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="I83" s="64"/>
-      <c r="J83" s="64"/>
-      <c r="K83" s="64"/>
-      <c r="L83" s="64"/>
-      <c r="M83" s="61" t="s">
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="65"/>
+      <c r="L83" s="65"/>
+      <c r="M83" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="N83" s="61"/>
-      <c r="O83" s="61" t="s">
+      <c r="N83" s="66"/>
+      <c r="O83" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="P83" s="61"/>
+      <c r="P83" s="66"/>
       <c r="Q83" s="33"/>
       <c r="R83" s="33"/>
     </row>
@@ -3866,13 +3867,13 @@
       <c r="E84" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H84" s="68" t="s">
+      <c r="H84" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="I84" s="68"/>
-      <c r="J84" s="68"/>
-      <c r="K84" s="68"/>
-      <c r="L84" s="68"/>
+      <c r="I84" s="67"/>
+      <c r="J84" s="67"/>
+      <c r="K84" s="67"/>
+      <c r="L84" s="67"/>
       <c r="M84" s="43" t="s">
         <v>64</v>
       </c>
@@ -3905,10 +3906,10 @@
       <c r="N85" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S85" s="63" t="s">
+      <c r="S85" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="T85" s="63"/>
+      <c r="T85" s="68"/>
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" s="34" t="s">
@@ -3923,22 +3924,22 @@
       <c r="J86" s="37"/>
       <c r="K86" s="32"/>
       <c r="L86" s="37"/>
-      <c r="N86" s="60" t="s">
+      <c r="N86" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="O86" s="60"/>
-      <c r="P86" s="60"/>
-      <c r="Q86" s="60"/>
-      <c r="R86" s="60"/>
-      <c r="S86" s="60" t="s">
+      <c r="O86" s="62"/>
+      <c r="P86" s="62"/>
+      <c r="Q86" s="62"/>
+      <c r="R86" s="62"/>
+      <c r="S86" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="T86" s="60"/>
-      <c r="U86" s="60"/>
-      <c r="V86" s="60"/>
-      <c r="W86" s="60"/>
-      <c r="X86" s="60"/>
-      <c r="Y86" s="60"/>
+      <c r="T86" s="62"/>
+      <c r="U86" s="62"/>
+      <c r="V86" s="62"/>
+      <c r="W86" s="62"/>
+      <c r="X86" s="62"/>
+      <c r="Y86" s="62"/>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
@@ -3961,22 +3962,22 @@
       <c r="J87" s="31"/>
       <c r="K87" s="37"/>
       <c r="L87" s="32"/>
-      <c r="N87" s="60" t="s">
+      <c r="N87" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="O87" s="60"/>
-      <c r="P87" s="60"/>
-      <c r="Q87" s="60"/>
-      <c r="R87" s="60"/>
-      <c r="S87" s="60" t="s">
+      <c r="O87" s="62"/>
+      <c r="P87" s="62"/>
+      <c r="Q87" s="62"/>
+      <c r="R87" s="62"/>
+      <c r="S87" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="T87" s="60"/>
-      <c r="U87" s="60"/>
-      <c r="V87" s="60"/>
-      <c r="W87" s="60"/>
-      <c r="X87" s="60"/>
-      <c r="Y87" s="60"/>
+      <c r="T87" s="62"/>
+      <c r="U87" s="62"/>
+      <c r="V87" s="62"/>
+      <c r="W87" s="62"/>
+      <c r="X87" s="62"/>
+      <c r="Y87" s="62"/>
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
@@ -3999,22 +4000,22 @@
       <c r="J88" s="31"/>
       <c r="K88" s="38"/>
       <c r="L88" s="37"/>
-      <c r="N88" s="60" t="s">
+      <c r="N88" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="O88" s="60"/>
-      <c r="P88" s="60"/>
-      <c r="Q88" s="60"/>
-      <c r="R88" s="60"/>
-      <c r="S88" s="60" t="s">
+      <c r="O88" s="62"/>
+      <c r="P88" s="62"/>
+      <c r="Q88" s="62"/>
+      <c r="R88" s="62"/>
+      <c r="S88" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="T88" s="60"/>
-      <c r="U88" s="60"/>
-      <c r="V88" s="60"/>
-      <c r="W88" s="60"/>
-      <c r="X88" s="60"/>
-      <c r="Y88" s="60"/>
+      <c r="T88" s="62"/>
+      <c r="U88" s="62"/>
+      <c r="V88" s="62"/>
+      <c r="W88" s="62"/>
+      <c r="X88" s="62"/>
+      <c r="Y88" s="62"/>
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H89" s="32"/>
@@ -4022,20 +4023,20 @@
       <c r="J89" s="38"/>
       <c r="K89" s="37"/>
       <c r="L89" s="32"/>
-      <c r="N89" s="60"/>
-      <c r="O89" s="60"/>
-      <c r="P89" s="60"/>
-      <c r="Q89" s="60"/>
-      <c r="R89" s="60"/>
-      <c r="S89" s="60" t="s">
+      <c r="N89" s="62"/>
+      <c r="O89" s="62"/>
+      <c r="P89" s="62"/>
+      <c r="Q89" s="62"/>
+      <c r="R89" s="62"/>
+      <c r="S89" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="T89" s="60"/>
-      <c r="U89" s="60"/>
-      <c r="V89" s="60"/>
-      <c r="W89" s="60"/>
-      <c r="X89" s="60"/>
-      <c r="Y89" s="60"/>
+      <c r="T89" s="62"/>
+      <c r="U89" s="62"/>
+      <c r="V89" s="62"/>
+      <c r="W89" s="62"/>
+      <c r="X89" s="62"/>
+      <c r="Y89" s="62"/>
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H90" s="37"/>
@@ -4043,37 +4044,167 @@
       <c r="J90" s="37"/>
       <c r="K90" s="32"/>
       <c r="L90" s="37"/>
-      <c r="N90" s="60"/>
-      <c r="O90" s="60"/>
-      <c r="P90" s="60"/>
-      <c r="Q90" s="60"/>
-      <c r="R90" s="60"/>
-      <c r="S90" s="60" t="s">
+      <c r="N90" s="62"/>
+      <c r="O90" s="62"/>
+      <c r="P90" s="62"/>
+      <c r="Q90" s="62"/>
+      <c r="R90" s="62"/>
+      <c r="S90" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="T90" s="60"/>
-      <c r="U90" s="60"/>
-      <c r="V90" s="60"/>
-      <c r="W90" s="60"/>
-      <c r="X90" s="60"/>
-      <c r="Y90" s="60"/>
+      <c r="T90" s="62"/>
+      <c r="U90" s="62"/>
+      <c r="V90" s="62"/>
+      <c r="W90" s="62"/>
+      <c r="X90" s="62"/>
+      <c r="Y90" s="62"/>
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N91" s="62"/>
-      <c r="O91" s="62"/>
-      <c r="P91" s="62"/>
-      <c r="Q91" s="62"/>
-      <c r="R91" s="62"/>
-      <c r="S91" s="62"/>
-      <c r="T91" s="62"/>
-      <c r="U91" s="62"/>
-      <c r="V91" s="62"/>
-      <c r="W91" s="62"/>
-      <c r="X91" s="62"/>
-      <c r="Y91" s="62"/>
+      <c r="N91" s="60"/>
+      <c r="O91" s="60"/>
+      <c r="P91" s="60"/>
+      <c r="Q91" s="60"/>
+      <c r="R91" s="60"/>
+      <c r="S91" s="60"/>
+      <c r="T91" s="60"/>
+      <c r="U91" s="60"/>
+      <c r="V91" s="60"/>
+      <c r="W91" s="60"/>
+      <c r="X91" s="60"/>
+      <c r="Y91" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="154">
+    <mergeCell ref="N75:R75"/>
+    <mergeCell ref="S75:Y75"/>
+    <mergeCell ref="N76:R76"/>
+    <mergeCell ref="S76:Y76"/>
+    <mergeCell ref="N77:R77"/>
+    <mergeCell ref="S77:Y77"/>
+    <mergeCell ref="O70:P70"/>
+    <mergeCell ref="N64:R64"/>
+    <mergeCell ref="S64:Y64"/>
+    <mergeCell ref="N65:R65"/>
+    <mergeCell ref="S65:Y65"/>
+    <mergeCell ref="N74:R74"/>
+    <mergeCell ref="S74:Y74"/>
+    <mergeCell ref="N61:R61"/>
+    <mergeCell ref="S61:Y61"/>
+    <mergeCell ref="N62:R62"/>
+    <mergeCell ref="S62:Y62"/>
+    <mergeCell ref="N63:R63"/>
+    <mergeCell ref="S63:Y63"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="S72:T72"/>
+    <mergeCell ref="N73:R73"/>
+    <mergeCell ref="S73:Y73"/>
+    <mergeCell ref="H67:L67"/>
+    <mergeCell ref="H68:L68"/>
+    <mergeCell ref="H69:L69"/>
+    <mergeCell ref="M69:N69"/>
+    <mergeCell ref="H70:L70"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="T69:U69"/>
+    <mergeCell ref="V69:W69"/>
+    <mergeCell ref="T68:U68"/>
+    <mergeCell ref="V68:W68"/>
+    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="M56:N56"/>
+    <mergeCell ref="H58:L58"/>
+    <mergeCell ref="S59:T59"/>
+    <mergeCell ref="N60:R60"/>
+    <mergeCell ref="S60:Y60"/>
+    <mergeCell ref="S48:Y48"/>
+    <mergeCell ref="S49:Y49"/>
+    <mergeCell ref="S50:Y50"/>
+    <mergeCell ref="N50:R50"/>
+    <mergeCell ref="H57:L57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="T55:U55"/>
+    <mergeCell ref="T56:U56"/>
+    <mergeCell ref="V55:W55"/>
+    <mergeCell ref="V56:W56"/>
+    <mergeCell ref="V57:W57"/>
+    <mergeCell ref="T57:U57"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="H54:L54"/>
+    <mergeCell ref="S36:Y36"/>
+    <mergeCell ref="S37:Y37"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="S45:Y45"/>
+    <mergeCell ref="S46:Y46"/>
+    <mergeCell ref="S47:Y47"/>
+    <mergeCell ref="S24:Y24"/>
+    <mergeCell ref="S25:Y25"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="S33:Y33"/>
+    <mergeCell ref="S34:Y34"/>
+    <mergeCell ref="S35:Y35"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="S9:Y9"/>
+    <mergeCell ref="S10:Y10"/>
+    <mergeCell ref="S11:Y11"/>
+    <mergeCell ref="S12:Y12"/>
+    <mergeCell ref="S13:Y13"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="N47:R47"/>
+    <mergeCell ref="N48:R48"/>
+    <mergeCell ref="N49:R49"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:Y21"/>
+    <mergeCell ref="S22:Y22"/>
+    <mergeCell ref="S23:Y23"/>
+    <mergeCell ref="N45:R45"/>
+    <mergeCell ref="N46:R46"/>
+    <mergeCell ref="N35:R35"/>
+    <mergeCell ref="N36:R36"/>
+    <mergeCell ref="N37:R37"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="N33:R33"/>
+    <mergeCell ref="N34:R34"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="N12:R12"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="H80:L80"/>
+    <mergeCell ref="H81:L81"/>
+    <mergeCell ref="T81:U81"/>
+    <mergeCell ref="V81:W81"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="N22:R22"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="N25:R25"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H16:L16"/>
     <mergeCell ref="N91:R91"/>
     <mergeCell ref="S91:Y91"/>
     <mergeCell ref="A78:B78"/>
@@ -4098,136 +4229,6 @@
     <mergeCell ref="S85:T85"/>
     <mergeCell ref="N78:R78"/>
     <mergeCell ref="S78:Y78"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="H80:L80"/>
-    <mergeCell ref="H81:L81"/>
-    <mergeCell ref="T81:U81"/>
-    <mergeCell ref="V81:W81"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="N22:R22"/>
-    <mergeCell ref="N23:R23"/>
-    <mergeCell ref="N24:R24"/>
-    <mergeCell ref="N25:R25"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="S9:Y9"/>
-    <mergeCell ref="S10:Y10"/>
-    <mergeCell ref="S11:Y11"/>
-    <mergeCell ref="S12:Y12"/>
-    <mergeCell ref="S13:Y13"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="N47:R47"/>
-    <mergeCell ref="N48:R48"/>
-    <mergeCell ref="N49:R49"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:Y21"/>
-    <mergeCell ref="S22:Y22"/>
-    <mergeCell ref="S23:Y23"/>
-    <mergeCell ref="N45:R45"/>
-    <mergeCell ref="N46:R46"/>
-    <mergeCell ref="N35:R35"/>
-    <mergeCell ref="N36:R36"/>
-    <mergeCell ref="N37:R37"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="N33:R33"/>
-    <mergeCell ref="N34:R34"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="N12:R12"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="H54:L54"/>
-    <mergeCell ref="S36:Y36"/>
-    <mergeCell ref="S37:Y37"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="S45:Y45"/>
-    <mergeCell ref="S46:Y46"/>
-    <mergeCell ref="S47:Y47"/>
-    <mergeCell ref="S24:Y24"/>
-    <mergeCell ref="S25:Y25"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="S33:Y33"/>
-    <mergeCell ref="S34:Y34"/>
-    <mergeCell ref="S35:Y35"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="H55:L55"/>
-    <mergeCell ref="H56:L56"/>
-    <mergeCell ref="M56:N56"/>
-    <mergeCell ref="H58:L58"/>
-    <mergeCell ref="S59:T59"/>
-    <mergeCell ref="N60:R60"/>
-    <mergeCell ref="S60:Y60"/>
-    <mergeCell ref="S48:Y48"/>
-    <mergeCell ref="S49:Y49"/>
-    <mergeCell ref="S50:Y50"/>
-    <mergeCell ref="N50:R50"/>
-    <mergeCell ref="H57:L57"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="T55:U55"/>
-    <mergeCell ref="T56:U56"/>
-    <mergeCell ref="V55:W55"/>
-    <mergeCell ref="V56:W56"/>
-    <mergeCell ref="V57:W57"/>
-    <mergeCell ref="T57:U57"/>
-    <mergeCell ref="N61:R61"/>
-    <mergeCell ref="S61:Y61"/>
-    <mergeCell ref="N62:R62"/>
-    <mergeCell ref="S62:Y62"/>
-    <mergeCell ref="N63:R63"/>
-    <mergeCell ref="S63:Y63"/>
-    <mergeCell ref="H71:L71"/>
-    <mergeCell ref="S72:T72"/>
-    <mergeCell ref="N73:R73"/>
-    <mergeCell ref="S73:Y73"/>
-    <mergeCell ref="H67:L67"/>
-    <mergeCell ref="H68:L68"/>
-    <mergeCell ref="H69:L69"/>
-    <mergeCell ref="M69:N69"/>
-    <mergeCell ref="H70:L70"/>
-    <mergeCell ref="M70:N70"/>
-    <mergeCell ref="T69:U69"/>
-    <mergeCell ref="V69:W69"/>
-    <mergeCell ref="T68:U68"/>
-    <mergeCell ref="V68:W68"/>
-    <mergeCell ref="N75:R75"/>
-    <mergeCell ref="S75:Y75"/>
-    <mergeCell ref="N76:R76"/>
-    <mergeCell ref="S76:Y76"/>
-    <mergeCell ref="N77:R77"/>
-    <mergeCell ref="S77:Y77"/>
-    <mergeCell ref="O70:P70"/>
-    <mergeCell ref="N64:R64"/>
-    <mergeCell ref="S64:Y64"/>
-    <mergeCell ref="N65:R65"/>
-    <mergeCell ref="S65:Y65"/>
-    <mergeCell ref="N74:R74"/>
-    <mergeCell ref="S74:Y74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>